<commit_message>
inserido o crud do cadastro de cliente
</commit_message>
<xml_diff>
--- a/documentação/Catalogo_Dados.xlsx
+++ b/documentação/Catalogo_Dados.xlsx
@@ -1,20 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23001"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\projetos\portal-mori-novo-dois\documentação\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\projetos\contabil_novo\documentação\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E14AF694-4F59-49E7-A77C-99BFC91B46B5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B05246E-57F3-4C02-AD93-589347648D51}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{BBCC3619-9FAE-4B62-80B6-86EE0ECD51E8}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{BBCC3619-9FAE-4B62-80B6-86EE0ECD51E8}"/>
   </bookViews>
   <sheets>
     <sheet name="aluno" sheetId="1" r:id="rId1"/>
     <sheet name="usuario" sheetId="2" r:id="rId2"/>
+    <sheet name="cliente" sheetId="3" r:id="rId3"/>
+    <sheet name="Planilha2" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="340" uniqueCount="120">
   <si>
     <t># id</t>
   </si>
@@ -277,6 +279,123 @@
   </si>
   <si>
     <t>admin</t>
+  </si>
+  <si>
+    <t># idCliente</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> cnpj</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> nome_fantasia</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> razao_social</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> cep</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> endereco</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> numero</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> bairro</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> cidade</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> uf</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> email</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> telefone</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> celular</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> contato</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> obs</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> dataCadastro</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> dataModificacao</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> idUsuario</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> cnpjClienteCadastro</t>
+  </si>
+  <si>
+    <t>'14'</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> '05.341.639/0001-54'</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'KEYRUS BRASIL'</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'KEYRUS BRASIL SERVICOS DE INFORMATICA LTDA.'</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> '01.310-100'</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'AV PAULISTA'</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> '1374'</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'BELA VISTA'</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'SAO PAULO'</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'SP'</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'financeiro@keyrus.com.br'</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> '(11) 5070-1400'</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'KEYRUS SA'</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'teste'</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> '2020-06-04 13:00:42'</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> '21'</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> '19.313.885/0001-07'</t>
+  </si>
+  <si>
+    <t>idCliente</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> nomeFantasia</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> razaoSocial</t>
   </si>
 </sst>
 </file>
@@ -2124,7 +2243,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C71ECD93-53B4-4613-8409-D1464380A165}">
   <dimension ref="A1:Z30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
@@ -2451,7 +2570,7 @@
         <v>$usuario-&gt;setidUnidade($_POST['idUnidade']);</v>
       </c>
     </row>
-    <row r="8" spans="1:26" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:26" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>66</v>
       </c>
@@ -2480,7 +2599,7 @@
         <v>$usuario-&gt;setcref($_POST['cref']);</v>
       </c>
     </row>
-    <row r="9" spans="1:26" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:26" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>1</v>
       </c>
@@ -2512,7 +2631,7 @@
         <v>$usuario-&gt;setnome($_POST['nome']);</v>
       </c>
     </row>
-    <row r="10" spans="1:26" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:26" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>2</v>
       </c>
@@ -2544,7 +2663,7 @@
         <v>$usuario-&gt;setdataNascimento($_POST['dataNascimento']);</v>
       </c>
     </row>
-    <row r="11" spans="1:26" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:26" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>3</v>
       </c>
@@ -2576,7 +2695,7 @@
         <v>$usuario-&gt;setcpf($_POST['cpf']);</v>
       </c>
     </row>
-    <row r="12" spans="1:26" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:26" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>4</v>
       </c>
@@ -2608,7 +2727,7 @@
         <v>$usuario-&gt;setrg($_POST['rg']);</v>
       </c>
     </row>
-    <row r="13" spans="1:26" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:26" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>5</v>
       </c>
@@ -2640,7 +2759,7 @@
         <v>$usuario-&gt;setsexo($_POST['sexo']);</v>
       </c>
     </row>
-    <row r="14" spans="1:26" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:26" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>6</v>
       </c>
@@ -2672,7 +2791,7 @@
         <v>$usuario-&gt;setcep($_POST['cep']);</v>
       </c>
     </row>
-    <row r="15" spans="1:26" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:26" ht="72" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>7</v>
       </c>
@@ -2704,7 +2823,7 @@
         <v>$usuario-&gt;setendereco($_POST['endereco']);</v>
       </c>
     </row>
-    <row r="16" spans="1:26" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:26" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>8</v>
       </c>
@@ -2768,7 +2887,7 @@
         <v>$usuario-&gt;setcidade($_POST['cidade']);</v>
       </c>
     </row>
-    <row r="18" spans="1:8" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>10</v>
       </c>
@@ -2800,7 +2919,7 @@
         <v>$usuario-&gt;setuf($_POST['uf']);</v>
       </c>
     </row>
-    <row r="19" spans="1:8" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:8" ht="72" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>11</v>
       </c>
@@ -2832,7 +2951,7 @@
         <v>$usuario-&gt;setnumero($_POST['numero']);</v>
       </c>
     </row>
-    <row r="20" spans="1:8" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:8" ht="72" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>12</v>
       </c>
@@ -2864,7 +2983,7 @@
         <v>$usuario-&gt;settelefone($_POST['telefone']);</v>
       </c>
     </row>
-    <row r="21" spans="1:8" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:8" ht="72" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>13</v>
       </c>
@@ -2896,7 +3015,7 @@
         <v>$usuario-&gt;setcelular($_POST['celular']);</v>
       </c>
     </row>
-    <row r="22" spans="1:8" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>14</v>
       </c>
@@ -2928,7 +3047,7 @@
         <v>$usuario-&gt;setemail($_POST['email']);</v>
       </c>
     </row>
-    <row r="23" spans="1:8" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:8" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>67</v>
       </c>
@@ -2960,7 +3079,7 @@
         <v>$usuario-&gt;setdataAdmissao($_POST['dataAdmissao']);</v>
       </c>
     </row>
-    <row r="24" spans="1:8" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:8" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>68</v>
       </c>
@@ -3024,7 +3143,7 @@
         <v>$usuario-&gt;setobservacao($_POST['observacao']);</v>
       </c>
     </row>
-    <row r="26" spans="1:8" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:8" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>24</v>
       </c>
@@ -3056,7 +3175,7 @@
         <v>$usuario-&gt;setdataCadastro($_POST['dataCadastro']);</v>
       </c>
     </row>
-    <row r="27" spans="1:8" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>25</v>
       </c>
@@ -3088,7 +3207,7 @@
         <v>$usuario-&gt;setstatus($_POST['status']);</v>
       </c>
     </row>
-    <row r="28" spans="1:8" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>69</v>
       </c>
@@ -3120,7 +3239,7 @@
         <v>$usuario-&gt;setlogin($_POST['login']);</v>
       </c>
     </row>
-    <row r="29" spans="1:8" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>70</v>
       </c>
@@ -3182,6 +3301,978 @@
       <c r="H30" t="str">
         <f t="shared" si="4"/>
         <v>$usuario-&gt;setdataModificacao($_POST['dataModificacao']);</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE604228-F7D0-4F33-8CBA-8211E4D066BF}">
+  <dimension ref="A1:Z30"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5:E23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="15" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.77734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="24.77734375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="51.109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="4.77734375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="22.6640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.21875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="2.88671875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="7.33203125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="15.21875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="22.109375" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="5.88671875" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="6" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="7" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="15.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>117</v>
+      </c>
+      <c r="B1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C1" t="s">
+        <v>118</v>
+      </c>
+      <c r="D1" t="s">
+        <v>119</v>
+      </c>
+      <c r="E1" t="s">
+        <v>85</v>
+      </c>
+      <c r="F1" t="s">
+        <v>86</v>
+      </c>
+      <c r="G1" t="s">
+        <v>87</v>
+      </c>
+      <c r="H1" t="s">
+        <v>88</v>
+      </c>
+      <c r="I1" t="s">
+        <v>89</v>
+      </c>
+      <c r="J1" t="s">
+        <v>90</v>
+      </c>
+      <c r="K1" t="s">
+        <v>91</v>
+      </c>
+      <c r="L1" t="s">
+        <v>92</v>
+      </c>
+      <c r="M1" t="s">
+        <v>93</v>
+      </c>
+      <c r="N1" t="s">
+        <v>94</v>
+      </c>
+      <c r="O1" t="s">
+        <v>95</v>
+      </c>
+      <c r="P1" t="s">
+        <v>96</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>97</v>
+      </c>
+      <c r="R1" t="s">
+        <v>98</v>
+      </c>
+      <c r="S1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="2" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>100</v>
+      </c>
+      <c r="B2" t="s">
+        <v>101</v>
+      </c>
+      <c r="C2" t="s">
+        <v>102</v>
+      </c>
+      <c r="D2" t="s">
+        <v>103</v>
+      </c>
+      <c r="E2" t="s">
+        <v>104</v>
+      </c>
+      <c r="F2" t="s">
+        <v>105</v>
+      </c>
+      <c r="G2" t="s">
+        <v>106</v>
+      </c>
+      <c r="H2" t="s">
+        <v>107</v>
+      </c>
+      <c r="I2" t="s">
+        <v>108</v>
+      </c>
+      <c r="J2" t="s">
+        <v>109</v>
+      </c>
+      <c r="K2" t="s">
+        <v>110</v>
+      </c>
+      <c r="L2" t="s">
+        <v>111</v>
+      </c>
+      <c r="M2" t="s">
+        <v>111</v>
+      </c>
+      <c r="N2" t="s">
+        <v>112</v>
+      </c>
+      <c r="O2" t="s">
+        <v>113</v>
+      </c>
+      <c r="P2" t="s">
+        <v>114</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>114</v>
+      </c>
+      <c r="R2" t="s">
+        <v>115</v>
+      </c>
+      <c r="S2" t="s">
+        <v>116</v>
+      </c>
+      <c r="V2" s="2"/>
+      <c r="Z2" s="2"/>
+    </row>
+    <row r="3" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="F3" s="1"/>
+      <c r="S3" s="1"/>
+      <c r="V3" s="2"/>
+      <c r="Z3" s="2"/>
+    </row>
+    <row r="4" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A4" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="5" spans="1:26" ht="72" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>117</v>
+      </c>
+      <c r="B5" t="s">
+        <v>100</v>
+      </c>
+      <c r="C5" t="str">
+        <f>"$"&amp;TRIM(A5)&amp;","</f>
+        <v>$idCliente,</v>
+      </c>
+      <c r="D5" s="4" t="str">
+        <f>"public function get"&amp;TRIM($A5)&amp;"(){
+		return $this-&gt;"&amp;TRIM($A5)&amp;";
+	}"</f>
+        <v>public function getidCliente(){
+		return $this-&gt;idCliente;
+	}</v>
+      </c>
+      <c r="E5" s="4" t="str">
+        <f>"public function set"&amp;TRIM($A5)&amp;"($"&amp;TRIM(A5)&amp;"){
+		$this-&gt;"&amp;TRIM($A5)&amp;" = $"&amp;TRIM(A5)&amp;";
+	}"</f>
+        <v>public function setidCliente($idCliente){
+		$this-&gt;idCliente = $idCliente;
+	}</v>
+      </c>
+      <c r="F5" t="str">
+        <f>"name="""&amp;A5&amp;""""</f>
+        <v>name="idCliente"</v>
+      </c>
+      <c r="H5" t="str">
+        <f>"$cliente-&gt;set"&amp;$A5&amp;"($_POST['"&amp;$A5&amp;"']);"</f>
+        <v>$cliente-&gt;setidCliente($_POST['idCliente']);</v>
+      </c>
+    </row>
+    <row r="6" spans="1:26" ht="72" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>82</v>
+      </c>
+      <c r="B6" t="s">
+        <v>101</v>
+      </c>
+      <c r="C6" t="str">
+        <f t="shared" ref="C6:C23" si="0">"$"&amp;TRIM(A6)&amp;","</f>
+        <v>$cnpj,</v>
+      </c>
+      <c r="D6" s="4" t="str">
+        <f t="shared" ref="D6:D23" si="1">"public function get"&amp;TRIM($A6)&amp;"(){
+		return $this-&gt;"&amp;TRIM($A6)&amp;";
+	}"</f>
+        <v>public function getcnpj(){
+		return $this-&gt;cnpj;
+	}</v>
+      </c>
+      <c r="E6" s="4" t="str">
+        <f t="shared" ref="E6:E23" si="2">"public function set"&amp;TRIM($A6)&amp;"($"&amp;TRIM(A6)&amp;"){
+		$this-&gt;"&amp;TRIM($A6)&amp;" = $"&amp;TRIM(A6)&amp;";
+	}"</f>
+        <v>public function setcnpj($cnpj){
+		$this-&gt;cnpj = $cnpj;
+	}</v>
+      </c>
+      <c r="F6" t="str">
+        <f t="shared" ref="F6:F30" si="3">"name="""&amp;A6&amp;""""</f>
+        <v>name=" cnpj"</v>
+      </c>
+      <c r="H6" t="str">
+        <f t="shared" ref="H6:H23" si="4">"$cliente-&gt;set"&amp;$A6&amp;"($_POST['"&amp;$A6&amp;"']);"</f>
+        <v>$cliente-&gt;set cnpj($_POST[' cnpj']);</v>
+      </c>
+    </row>
+    <row r="7" spans="1:26" ht="72" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>118</v>
+      </c>
+      <c r="B7" t="s">
+        <v>102</v>
+      </c>
+      <c r="C7" t="str">
+        <f t="shared" si="0"/>
+        <v>$nomeFantasia,</v>
+      </c>
+      <c r="D7" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v>public function getnomeFantasia(){
+		return $this-&gt;nomeFantasia;
+	}</v>
+      </c>
+      <c r="E7" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v>public function setnomeFantasia($nomeFantasia){
+		$this-&gt;nomeFantasia = $nomeFantasia;
+	}</v>
+      </c>
+      <c r="F7" t="str">
+        <f t="shared" si="3"/>
+        <v>name=" nomeFantasia"</v>
+      </c>
+      <c r="H7" t="str">
+        <f t="shared" si="4"/>
+        <v>$cliente-&gt;set nomeFantasia($_POST[' nomeFantasia']);</v>
+      </c>
+    </row>
+    <row r="8" spans="1:26" ht="72" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>119</v>
+      </c>
+      <c r="B8" t="s">
+        <v>103</v>
+      </c>
+      <c r="C8" t="str">
+        <f t="shared" si="0"/>
+        <v>$razaoSocial,</v>
+      </c>
+      <c r="D8" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v>public function getrazaoSocial(){
+		return $this-&gt;razaoSocial;
+	}</v>
+      </c>
+      <c r="E8" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v>public function setrazaoSocial($razaoSocial){
+		$this-&gt;razaoSocial = $razaoSocial;
+	}</v>
+      </c>
+      <c r="F8" t="str">
+        <f t="shared" si="3"/>
+        <v>name=" razaoSocial"</v>
+      </c>
+      <c r="H8" t="str">
+        <f t="shared" si="4"/>
+        <v>$cliente-&gt;set razaoSocial($_POST[' razaoSocial']);</v>
+      </c>
+    </row>
+    <row r="9" spans="1:26" ht="72" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>85</v>
+      </c>
+      <c r="B9" t="s">
+        <v>104</v>
+      </c>
+      <c r="C9" t="str">
+        <f t="shared" si="0"/>
+        <v>$cep,</v>
+      </c>
+      <c r="D9" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v>public function getcep(){
+		return $this-&gt;cep;
+	}</v>
+      </c>
+      <c r="E9" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v>public function setcep($cep){
+		$this-&gt;cep = $cep;
+	}</v>
+      </c>
+      <c r="F9" t="str">
+        <f t="shared" si="3"/>
+        <v>name=" cep"</v>
+      </c>
+      <c r="H9" t="str">
+        <f t="shared" si="4"/>
+        <v>$cliente-&gt;set cep($_POST[' cep']);</v>
+      </c>
+    </row>
+    <row r="10" spans="1:26" ht="72" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>86</v>
+      </c>
+      <c r="B10" t="s">
+        <v>105</v>
+      </c>
+      <c r="C10" t="str">
+        <f t="shared" si="0"/>
+        <v>$endereco,</v>
+      </c>
+      <c r="D10" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v>public function getendereco(){
+		return $this-&gt;endereco;
+	}</v>
+      </c>
+      <c r="E10" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v>public function setendereco($endereco){
+		$this-&gt;endereco = $endereco;
+	}</v>
+      </c>
+      <c r="F10" t="str">
+        <f t="shared" si="3"/>
+        <v>name=" endereco"</v>
+      </c>
+      <c r="H10" t="str">
+        <f t="shared" si="4"/>
+        <v>$cliente-&gt;set endereco($_POST[' endereco']);</v>
+      </c>
+    </row>
+    <row r="11" spans="1:26" ht="72" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>87</v>
+      </c>
+      <c r="B11" t="s">
+        <v>106</v>
+      </c>
+      <c r="C11" t="str">
+        <f t="shared" si="0"/>
+        <v>$numero,</v>
+      </c>
+      <c r="D11" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v>public function getnumero(){
+		return $this-&gt;numero;
+	}</v>
+      </c>
+      <c r="E11" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v>public function setnumero($numero){
+		$this-&gt;numero = $numero;
+	}</v>
+      </c>
+      <c r="F11" t="str">
+        <f t="shared" si="3"/>
+        <v>name=" numero"</v>
+      </c>
+      <c r="H11" t="str">
+        <f t="shared" si="4"/>
+        <v>$cliente-&gt;set numero($_POST[' numero']);</v>
+      </c>
+    </row>
+    <row r="12" spans="1:26" ht="72" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>88</v>
+      </c>
+      <c r="B12" t="s">
+        <v>107</v>
+      </c>
+      <c r="C12" t="str">
+        <f t="shared" si="0"/>
+        <v>$bairro,</v>
+      </c>
+      <c r="D12" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v>public function getbairro(){
+		return $this-&gt;bairro;
+	}</v>
+      </c>
+      <c r="E12" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v>public function setbairro($bairro){
+		$this-&gt;bairro = $bairro;
+	}</v>
+      </c>
+      <c r="F12" t="str">
+        <f t="shared" si="3"/>
+        <v>name=" bairro"</v>
+      </c>
+      <c r="H12" t="str">
+        <f t="shared" si="4"/>
+        <v>$cliente-&gt;set bairro($_POST[' bairro']);</v>
+      </c>
+    </row>
+    <row r="13" spans="1:26" ht="72" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>89</v>
+      </c>
+      <c r="B13" t="s">
+        <v>108</v>
+      </c>
+      <c r="C13" t="str">
+        <f t="shared" si="0"/>
+        <v>$cidade,</v>
+      </c>
+      <c r="D13" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v>public function getcidade(){
+		return $this-&gt;cidade;
+	}</v>
+      </c>
+      <c r="E13" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v>public function setcidade($cidade){
+		$this-&gt;cidade = $cidade;
+	}</v>
+      </c>
+      <c r="F13" t="str">
+        <f t="shared" si="3"/>
+        <v>name=" cidade"</v>
+      </c>
+      <c r="H13" t="str">
+        <f t="shared" si="4"/>
+        <v>$cliente-&gt;set cidade($_POST[' cidade']);</v>
+      </c>
+    </row>
+    <row r="14" spans="1:26" ht="72" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>90</v>
+      </c>
+      <c r="B14" t="s">
+        <v>109</v>
+      </c>
+      <c r="C14" t="str">
+        <f t="shared" si="0"/>
+        <v>$uf,</v>
+      </c>
+      <c r="D14" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v>public function getuf(){
+		return $this-&gt;uf;
+	}</v>
+      </c>
+      <c r="E14" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v>public function setuf($uf){
+		$this-&gt;uf = $uf;
+	}</v>
+      </c>
+      <c r="F14" t="str">
+        <f t="shared" si="3"/>
+        <v>name=" uf"</v>
+      </c>
+      <c r="H14" t="str">
+        <f t="shared" si="4"/>
+        <v>$cliente-&gt;set uf($_POST[' uf']);</v>
+      </c>
+    </row>
+    <row r="15" spans="1:26" ht="72" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>91</v>
+      </c>
+      <c r="B15" t="s">
+        <v>110</v>
+      </c>
+      <c r="C15" t="str">
+        <f t="shared" si="0"/>
+        <v>$email,</v>
+      </c>
+      <c r="D15" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v>public function getemail(){
+		return $this-&gt;email;
+	}</v>
+      </c>
+      <c r="E15" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v>public function setemail($email){
+		$this-&gt;email = $email;
+	}</v>
+      </c>
+      <c r="F15" t="str">
+        <f t="shared" si="3"/>
+        <v>name=" email"</v>
+      </c>
+      <c r="H15" t="str">
+        <f t="shared" si="4"/>
+        <v>$cliente-&gt;set email($_POST[' email']);</v>
+      </c>
+    </row>
+    <row r="16" spans="1:26" ht="72" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>92</v>
+      </c>
+      <c r="B16" t="s">
+        <v>111</v>
+      </c>
+      <c r="C16" t="str">
+        <f t="shared" si="0"/>
+        <v>$telefone,</v>
+      </c>
+      <c r="D16" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v>public function gettelefone(){
+		return $this-&gt;telefone;
+	}</v>
+      </c>
+      <c r="E16" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v>public function settelefone($telefone){
+		$this-&gt;telefone = $telefone;
+	}</v>
+      </c>
+      <c r="F16" t="str">
+        <f t="shared" si="3"/>
+        <v>name=" telefone"</v>
+      </c>
+      <c r="H16" t="str">
+        <f t="shared" si="4"/>
+        <v>$cliente-&gt;set telefone($_POST[' telefone']);</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="72" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>93</v>
+      </c>
+      <c r="B17" t="s">
+        <v>111</v>
+      </c>
+      <c r="C17" t="str">
+        <f t="shared" si="0"/>
+        <v>$celular,</v>
+      </c>
+      <c r="D17" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v>public function getcelular(){
+		return $this-&gt;celular;
+	}</v>
+      </c>
+      <c r="E17" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v>public function setcelular($celular){
+		$this-&gt;celular = $celular;
+	}</v>
+      </c>
+      <c r="F17" t="str">
+        <f t="shared" si="3"/>
+        <v>name=" celular"</v>
+      </c>
+      <c r="H17" t="str">
+        <f t="shared" si="4"/>
+        <v>$cliente-&gt;set celular($_POST[' celular']);</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="72" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>94</v>
+      </c>
+      <c r="B18" t="s">
+        <v>112</v>
+      </c>
+      <c r="C18" t="str">
+        <f t="shared" si="0"/>
+        <v>$contato,</v>
+      </c>
+      <c r="D18" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v>public function getcontato(){
+		return $this-&gt;contato;
+	}</v>
+      </c>
+      <c r="E18" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v>public function setcontato($contato){
+		$this-&gt;contato = $contato;
+	}</v>
+      </c>
+      <c r="F18" t="str">
+        <f t="shared" si="3"/>
+        <v>name=" contato"</v>
+      </c>
+      <c r="H18" t="str">
+        <f t="shared" si="4"/>
+        <v>$cliente-&gt;set contato($_POST[' contato']);</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="72" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>95</v>
+      </c>
+      <c r="B19" t="s">
+        <v>113</v>
+      </c>
+      <c r="C19" t="str">
+        <f t="shared" si="0"/>
+        <v>$obs,</v>
+      </c>
+      <c r="D19" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v>public function getobs(){
+		return $this-&gt;obs;
+	}</v>
+      </c>
+      <c r="E19" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v>public function setobs($obs){
+		$this-&gt;obs = $obs;
+	}</v>
+      </c>
+      <c r="F19" t="str">
+        <f t="shared" si="3"/>
+        <v>name=" obs"</v>
+      </c>
+      <c r="H19" t="str">
+        <f t="shared" si="4"/>
+        <v>$cliente-&gt;set obs($_POST[' obs']);</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="72" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>96</v>
+      </c>
+      <c r="B20" t="s">
+        <v>114</v>
+      </c>
+      <c r="C20" t="str">
+        <f t="shared" si="0"/>
+        <v>$dataCadastro,</v>
+      </c>
+      <c r="D20" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v>public function getdataCadastro(){
+		return $this-&gt;dataCadastro;
+	}</v>
+      </c>
+      <c r="E20" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v>public function setdataCadastro($dataCadastro){
+		$this-&gt;dataCadastro = $dataCadastro;
+	}</v>
+      </c>
+      <c r="F20" t="str">
+        <f t="shared" si="3"/>
+        <v>name=" dataCadastro"</v>
+      </c>
+      <c r="H20" t="str">
+        <f t="shared" si="4"/>
+        <v>$cliente-&gt;set dataCadastro($_POST[' dataCadastro']);</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="72" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>97</v>
+      </c>
+      <c r="B21" t="s">
+        <v>114</v>
+      </c>
+      <c r="C21" t="str">
+        <f t="shared" si="0"/>
+        <v>$dataModificacao,</v>
+      </c>
+      <c r="D21" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v>public function getdataModificacao(){
+		return $this-&gt;dataModificacao;
+	}</v>
+      </c>
+      <c r="E21" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v>public function setdataModificacao($dataModificacao){
+		$this-&gt;dataModificacao = $dataModificacao;
+	}</v>
+      </c>
+      <c r="F21" t="str">
+        <f t="shared" si="3"/>
+        <v>name=" dataModificacao"</v>
+      </c>
+      <c r="H21" t="str">
+        <f t="shared" si="4"/>
+        <v>$cliente-&gt;set dataModificacao($_POST[' dataModificacao']);</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" ht="72" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>98</v>
+      </c>
+      <c r="B22" t="s">
+        <v>115</v>
+      </c>
+      <c r="C22" t="str">
+        <f t="shared" si="0"/>
+        <v>$idUsuario,</v>
+      </c>
+      <c r="D22" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v>public function getidUsuario(){
+		return $this-&gt;idUsuario;
+	}</v>
+      </c>
+      <c r="E22" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v>public function setidUsuario($idUsuario){
+		$this-&gt;idUsuario = $idUsuario;
+	}</v>
+      </c>
+      <c r="F22" t="str">
+        <f t="shared" si="3"/>
+        <v>name=" idUsuario"</v>
+      </c>
+      <c r="H22" t="str">
+        <f t="shared" si="4"/>
+        <v>$cliente-&gt;set idUsuario($_POST[' idUsuario']);</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>99</v>
+      </c>
+      <c r="B23" t="s">
+        <v>116</v>
+      </c>
+      <c r="C23" t="str">
+        <f t="shared" si="0"/>
+        <v>$cnpjClienteCadastro,</v>
+      </c>
+      <c r="D23" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v>public function getcnpjClienteCadastro(){
+		return $this-&gt;cnpjClienteCadastro;
+	}</v>
+      </c>
+      <c r="E23" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v>public function setcnpjClienteCadastro($cnpjClienteCadastro){
+		$this-&gt;cnpjClienteCadastro = $cnpjClienteCadastro;
+	}</v>
+      </c>
+      <c r="F23" t="str">
+        <f t="shared" si="3"/>
+        <v>name=" cnpjClienteCadastro"</v>
+      </c>
+      <c r="H23" t="str">
+        <f t="shared" si="4"/>
+        <v>$cliente-&gt;set cnpjClienteCadastro($_POST[' cnpjClienteCadastro']);</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="D24" s="4"/>
+      <c r="E24" s="4"/>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="D25" s="4"/>
+      <c r="E25" s="4"/>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="D26" s="4"/>
+      <c r="E26" s="4"/>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="D27" s="4"/>
+      <c r="E27" s="4"/>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="D28" s="4"/>
+      <c r="E28" s="4"/>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="D29" s="4"/>
+      <c r="E29" s="4"/>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="D30" s="4"/>
+      <c r="E30" s="4"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27F77242-1B9B-47EA-8A4A-62F783FD6B77}">
+  <dimension ref="A1:S2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:S2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C1" t="s">
+        <v>83</v>
+      </c>
+      <c r="D1" t="s">
+        <v>84</v>
+      </c>
+      <c r="E1" t="s">
+        <v>85</v>
+      </c>
+      <c r="F1" t="s">
+        <v>86</v>
+      </c>
+      <c r="G1" t="s">
+        <v>87</v>
+      </c>
+      <c r="H1" t="s">
+        <v>88</v>
+      </c>
+      <c r="I1" t="s">
+        <v>89</v>
+      </c>
+      <c r="J1" t="s">
+        <v>90</v>
+      </c>
+      <c r="K1" t="s">
+        <v>91</v>
+      </c>
+      <c r="L1" t="s">
+        <v>92</v>
+      </c>
+      <c r="M1" t="s">
+        <v>93</v>
+      </c>
+      <c r="N1" t="s">
+        <v>94</v>
+      </c>
+      <c r="O1" t="s">
+        <v>95</v>
+      </c>
+      <c r="P1" t="s">
+        <v>96</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>97</v>
+      </c>
+      <c r="R1" t="s">
+        <v>98</v>
+      </c>
+      <c r="S1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>100</v>
+      </c>
+      <c r="B2" t="s">
+        <v>101</v>
+      </c>
+      <c r="C2" t="s">
+        <v>102</v>
+      </c>
+      <c r="D2" t="s">
+        <v>103</v>
+      </c>
+      <c r="E2" t="s">
+        <v>104</v>
+      </c>
+      <c r="F2" t="s">
+        <v>105</v>
+      </c>
+      <c r="G2" t="s">
+        <v>106</v>
+      </c>
+      <c r="H2" t="s">
+        <v>107</v>
+      </c>
+      <c r="I2" t="s">
+        <v>108</v>
+      </c>
+      <c r="J2" t="s">
+        <v>109</v>
+      </c>
+      <c r="K2" t="s">
+        <v>110</v>
+      </c>
+      <c r="L2" t="s">
+        <v>111</v>
+      </c>
+      <c r="M2" t="s">
+        <v>111</v>
+      </c>
+      <c r="N2" t="s">
+        <v>112</v>
+      </c>
+      <c r="O2" t="s">
+        <v>113</v>
+      </c>
+      <c r="P2" t="s">
+        <v>114</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>114</v>
+      </c>
+      <c r="R2" t="s">
+        <v>115</v>
+      </c>
+      <c r="S2" t="s">
+        <v>116</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
inserido o crud do cadastro de servico
</commit_message>
<xml_diff>
--- a/documentação/Catalogo_Dados.xlsx
+++ b/documentação/Catalogo_Dados.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\projetos\contabil_novo\documentação\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B05246E-57F3-4C02-AD93-589347648D51}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD92E6D5-7CFF-462A-A683-E058B8B79343}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{BBCC3619-9FAE-4B62-80B6-86EE0ECD51E8}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{BBCC3619-9FAE-4B62-80B6-86EE0ECD51E8}"/>
   </bookViews>
   <sheets>
     <sheet name="aluno" sheetId="1" r:id="rId1"/>
     <sheet name="usuario" sheetId="2" r:id="rId2"/>
     <sheet name="cliente" sheetId="3" r:id="rId3"/>
-    <sheet name="Planilha2" sheetId="4" r:id="rId4"/>
+    <sheet name="servico" sheetId="5" r:id="rId4"/>
+    <sheet name="Planilha2" sheetId="4" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="340" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="346" uniqueCount="126">
   <si>
     <t># id</t>
   </si>
@@ -281,18 +282,9 @@
     <t>admin</t>
   </si>
   <si>
-    <t># idCliente</t>
-  </si>
-  <si>
     <t xml:space="preserve"> cnpj</t>
   </si>
   <si>
-    <t xml:space="preserve"> nome_fantasia</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> razao_social</t>
-  </si>
-  <si>
     <t xml:space="preserve"> cep</t>
   </si>
   <si>
@@ -396,6 +388,33 @@
   </si>
   <si>
     <t xml:space="preserve"> razaoSocial</t>
+  </si>
+  <si>
+    <t># idServico</t>
+  </si>
+  <si>
+    <t>servico</t>
+  </si>
+  <si>
+    <t>tipo</t>
+  </si>
+  <si>
+    <t>descricao</t>
+  </si>
+  <si>
+    <t>cnpjClienteCadastro</t>
+  </si>
+  <si>
+    <t>Financeiro</t>
+  </si>
+  <si>
+    <t>Administrativo</t>
+  </si>
+  <si>
+    <t>Treinamento</t>
+  </si>
+  <si>
+    <t>19.313.885/0001-07</t>
   </si>
 </sst>
 </file>
@@ -3312,7 +3331,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE604228-F7D0-4F33-8CBA-8211E4D066BF}">
   <dimension ref="A1:Z30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+    <sheetView topLeftCell="A20" workbookViewId="0">
       <selection activeCell="E5" sqref="E5:E23"/>
     </sheetView>
   </sheetViews>
@@ -3348,120 +3367,120 @@
   <sheetData>
     <row r="1" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="B1" t="s">
+        <v>81</v>
+      </c>
+      <c r="C1" t="s">
+        <v>115</v>
+      </c>
+      <c r="D1" t="s">
+        <v>116</v>
+      </c>
+      <c r="E1" t="s">
         <v>82</v>
       </c>
-      <c r="C1" t="s">
-        <v>118</v>
-      </c>
-      <c r="D1" t="s">
-        <v>119</v>
-      </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
+        <v>83</v>
+      </c>
+      <c r="G1" t="s">
+        <v>84</v>
+      </c>
+      <c r="H1" t="s">
         <v>85</v>
       </c>
-      <c r="F1" t="s">
+      <c r="I1" t="s">
         <v>86</v>
       </c>
-      <c r="G1" t="s">
+      <c r="J1" t="s">
         <v>87</v>
       </c>
-      <c r="H1" t="s">
+      <c r="K1" t="s">
         <v>88</v>
       </c>
-      <c r="I1" t="s">
+      <c r="L1" t="s">
         <v>89</v>
       </c>
-      <c r="J1" t="s">
+      <c r="M1" t="s">
         <v>90</v>
       </c>
-      <c r="K1" t="s">
+      <c r="N1" t="s">
         <v>91</v>
       </c>
-      <c r="L1" t="s">
+      <c r="O1" t="s">
         <v>92</v>
       </c>
-      <c r="M1" t="s">
+      <c r="P1" t="s">
         <v>93</v>
       </c>
-      <c r="N1" t="s">
+      <c r="Q1" t="s">
         <v>94</v>
       </c>
-      <c r="O1" t="s">
+      <c r="R1" t="s">
         <v>95</v>
       </c>
-      <c r="P1" t="s">
+      <c r="S1" t="s">
         <v>96</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>97</v>
-      </c>
-      <c r="R1" t="s">
-        <v>98</v>
-      </c>
-      <c r="S1" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>97</v>
+      </c>
+      <c r="B2" t="s">
+        <v>98</v>
+      </c>
+      <c r="C2" t="s">
+        <v>99</v>
+      </c>
+      <c r="D2" t="s">
         <v>100</v>
       </c>
-      <c r="B2" t="s">
+      <c r="E2" t="s">
         <v>101</v>
       </c>
-      <c r="C2" t="s">
+      <c r="F2" t="s">
         <v>102</v>
       </c>
-      <c r="D2" t="s">
+      <c r="G2" t="s">
         <v>103</v>
       </c>
-      <c r="E2" t="s">
+      <c r="H2" t="s">
         <v>104</v>
       </c>
-      <c r="F2" t="s">
+      <c r="I2" t="s">
         <v>105</v>
       </c>
-      <c r="G2" t="s">
+      <c r="J2" t="s">
         <v>106</v>
       </c>
-      <c r="H2" t="s">
+      <c r="K2" t="s">
         <v>107</v>
       </c>
-      <c r="I2" t="s">
+      <c r="L2" t="s">
         <v>108</v>
       </c>
-      <c r="J2" t="s">
+      <c r="M2" t="s">
+        <v>108</v>
+      </c>
+      <c r="N2" t="s">
         <v>109</v>
       </c>
-      <c r="K2" t="s">
+      <c r="O2" t="s">
         <v>110</v>
       </c>
-      <c r="L2" t="s">
+      <c r="P2" t="s">
         <v>111</v>
       </c>
-      <c r="M2" t="s">
+      <c r="Q2" t="s">
         <v>111</v>
       </c>
-      <c r="N2" t="s">
+      <c r="R2" t="s">
         <v>112</v>
       </c>
-      <c r="O2" t="s">
+      <c r="S2" t="s">
         <v>113</v>
-      </c>
-      <c r="P2" t="s">
-        <v>114</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>114</v>
-      </c>
-      <c r="R2" t="s">
-        <v>115</v>
-      </c>
-      <c r="S2" t="s">
-        <v>116</v>
       </c>
       <c r="V2" s="2"/>
       <c r="Z2" s="2"/>
@@ -3500,10 +3519,10 @@
     </row>
     <row r="5" spans="1:26" ht="72" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="B5" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="C5" t="str">
         <f>"$"&amp;TRIM(A5)&amp;","</f>
@@ -3536,10 +3555,10 @@
     </row>
     <row r="6" spans="1:26" ht="72" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B6" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="C6" t="str">
         <f t="shared" ref="C6:C23" si="0">"$"&amp;TRIM(A6)&amp;","</f>
@@ -3562,7 +3581,7 @@
 	}</v>
       </c>
       <c r="F6" t="str">
-        <f t="shared" ref="F6:F30" si="3">"name="""&amp;A6&amp;""""</f>
+        <f t="shared" ref="F6:F23" si="3">"name="""&amp;A6&amp;""""</f>
         <v>name=" cnpj"</v>
       </c>
       <c r="H6" t="str">
@@ -3572,10 +3591,10 @@
     </row>
     <row r="7" spans="1:26" ht="72" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="B7" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="C7" t="str">
         <f t="shared" si="0"/>
@@ -3604,10 +3623,10 @@
     </row>
     <row r="8" spans="1:26" ht="72" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="B8" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="C8" t="str">
         <f t="shared" si="0"/>
@@ -3636,10 +3655,10 @@
     </row>
     <row r="9" spans="1:26" ht="72" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="B9" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="C9" t="str">
         <f t="shared" si="0"/>
@@ -3668,10 +3687,10 @@
     </row>
     <row r="10" spans="1:26" ht="72" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="B10" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="C10" t="str">
         <f t="shared" si="0"/>
@@ -3700,10 +3719,10 @@
     </row>
     <row r="11" spans="1:26" ht="72" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="B11" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="C11" t="str">
         <f t="shared" si="0"/>
@@ -3732,10 +3751,10 @@
     </row>
     <row r="12" spans="1:26" ht="72" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="B12" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="C12" t="str">
         <f t="shared" si="0"/>
@@ -3764,10 +3783,10 @@
     </row>
     <row r="13" spans="1:26" ht="72" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="B13" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="C13" t="str">
         <f t="shared" si="0"/>
@@ -3796,10 +3815,10 @@
     </row>
     <row r="14" spans="1:26" ht="72" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="B14" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="C14" t="str">
         <f t="shared" si="0"/>
@@ -3828,10 +3847,10 @@
     </row>
     <row r="15" spans="1:26" ht="72" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="B15" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="C15" t="str">
         <f t="shared" si="0"/>
@@ -3860,10 +3879,10 @@
     </row>
     <row r="16" spans="1:26" ht="72" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="B16" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="C16" t="str">
         <f t="shared" si="0"/>
@@ -3892,10 +3911,10 @@
     </row>
     <row r="17" spans="1:8" ht="72" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="B17" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="C17" t="str">
         <f t="shared" si="0"/>
@@ -3924,10 +3943,10 @@
     </row>
     <row r="18" spans="1:8" ht="72" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="B18" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="C18" t="str">
         <f t="shared" si="0"/>
@@ -3956,10 +3975,10 @@
     </row>
     <row r="19" spans="1:8" ht="72" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="B19" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="C19" t="str">
         <f t="shared" si="0"/>
@@ -3988,10 +4007,10 @@
     </row>
     <row r="20" spans="1:8" ht="72" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="B20" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="C20" t="str">
         <f t="shared" si="0"/>
@@ -4020,10 +4039,10 @@
     </row>
     <row r="21" spans="1:8" ht="72" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="B21" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="C21" t="str">
         <f t="shared" si="0"/>
@@ -4052,10 +4071,10 @@
     </row>
     <row r="22" spans="1:8" ht="72" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="B22" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="C22" t="str">
         <f t="shared" si="0"/>
@@ -4084,10 +4103,10 @@
     </row>
     <row r="23" spans="1:8" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="B23" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="C23" t="str">
         <f t="shared" si="0"/>
@@ -4148,131 +4167,530 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68FFEDBE-4954-4567-A0F1-2F9B239AEB62}">
+  <dimension ref="A1:Z30"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="15" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.77734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="24.77734375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="51.109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="4.77734375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="22.6640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.21875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="2.88671875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="7.33203125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="15.21875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="22.109375" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="5.88671875" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="6" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="7" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="15.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B1" t="s">
+        <v>118</v>
+      </c>
+      <c r="C1" t="s">
+        <v>119</v>
+      </c>
+      <c r="D1" t="s">
+        <v>120</v>
+      </c>
+      <c r="E1" t="s">
+        <v>121</v>
+      </c>
+      <c r="F1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G1" t="s">
+        <v>26</v>
+      </c>
+      <c r="H1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>18</v>
+      </c>
+      <c r="B2" t="s">
+        <v>122</v>
+      </c>
+      <c r="C2" t="s">
+        <v>123</v>
+      </c>
+      <c r="D2" t="s">
+        <v>124</v>
+      </c>
+      <c r="E2" t="s">
+        <v>125</v>
+      </c>
+      <c r="F2" s="2">
+        <v>43986.545439814814</v>
+      </c>
+      <c r="G2" s="2">
+        <v>43986.545439814814</v>
+      </c>
+      <c r="H2">
+        <v>22</v>
+      </c>
+      <c r="V2" s="2"/>
+      <c r="Z2" s="2"/>
+    </row>
+    <row r="3" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="F3" s="1"/>
+      <c r="S3" s="1"/>
+      <c r="V3" s="2"/>
+      <c r="Z3" s="2"/>
+    </row>
+    <row r="4" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A4" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="5" spans="1:26" ht="72" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>57</v>
+      </c>
+      <c r="B5">
+        <v>18</v>
+      </c>
+      <c r="C5" t="str">
+        <f>"$"&amp;TRIM(A5)&amp;","</f>
+        <v>$id,</v>
+      </c>
+      <c r="D5" s="4" t="str">
+        <f>"public function get"&amp;TRIM($A5)&amp;"(){
+		return $this-&gt;"&amp;TRIM($A5)&amp;";
+	}"</f>
+        <v>public function getid(){
+		return $this-&gt;id;
+	}</v>
+      </c>
+      <c r="E5" s="4" t="str">
+        <f>"public function set"&amp;TRIM($A5)&amp;"($"&amp;TRIM(A5)&amp;"){
+		$this-&gt;"&amp;TRIM($A5)&amp;" = $"&amp;TRIM(A5)&amp;";
+	}"</f>
+        <v>public function setid($id){
+		$this-&gt;id = $id;
+	}</v>
+      </c>
+      <c r="F5" t="str">
+        <f>"name="""&amp;A5&amp;""""</f>
+        <v>name="id"</v>
+      </c>
+      <c r="H5" t="str">
+        <f>"$servico-&gt;set"&amp;$A5&amp;"($_POST['"&amp;$A5&amp;"']);"</f>
+        <v>$servico-&gt;setid($_POST['id']);</v>
+      </c>
+    </row>
+    <row r="6" spans="1:26" ht="72" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>118</v>
+      </c>
+      <c r="B6" t="s">
+        <v>122</v>
+      </c>
+      <c r="C6" t="str">
+        <f t="shared" ref="C6:C23" si="0">"$"&amp;TRIM(A6)&amp;","</f>
+        <v>$servico,</v>
+      </c>
+      <c r="D6" s="4" t="str">
+        <f t="shared" ref="D6:D23" si="1">"public function get"&amp;TRIM($A6)&amp;"(){
+		return $this-&gt;"&amp;TRIM($A6)&amp;";
+	}"</f>
+        <v>public function getservico(){
+		return $this-&gt;servico;
+	}</v>
+      </c>
+      <c r="E6" s="4" t="str">
+        <f t="shared" ref="E6:E23" si="2">"public function set"&amp;TRIM($A6)&amp;"($"&amp;TRIM(A6)&amp;"){
+		$this-&gt;"&amp;TRIM($A6)&amp;" = $"&amp;TRIM(A6)&amp;";
+	}"</f>
+        <v>public function setservico($servico){
+		$this-&gt;servico = $servico;
+	}</v>
+      </c>
+      <c r="F6" t="str">
+        <f t="shared" ref="F6:F23" si="3">"name="""&amp;A6&amp;""""</f>
+        <v>name="servico"</v>
+      </c>
+      <c r="H6" t="str">
+        <f t="shared" ref="H6:H12" si="4">"$servico-&gt;set"&amp;$A6&amp;"($_POST['"&amp;$A6&amp;"']);"</f>
+        <v>$servico-&gt;setservico($_POST['servico']);</v>
+      </c>
+    </row>
+    <row r="7" spans="1:26" ht="72" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>119</v>
+      </c>
+      <c r="B7" t="s">
+        <v>123</v>
+      </c>
+      <c r="C7" t="str">
+        <f t="shared" si="0"/>
+        <v>$tipo,</v>
+      </c>
+      <c r="D7" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v>public function gettipo(){
+		return $this-&gt;tipo;
+	}</v>
+      </c>
+      <c r="E7" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v>public function settipo($tipo){
+		$this-&gt;tipo = $tipo;
+	}</v>
+      </c>
+      <c r="F7" t="str">
+        <f t="shared" si="3"/>
+        <v>name="tipo"</v>
+      </c>
+      <c r="H7" t="str">
+        <f t="shared" si="4"/>
+        <v>$servico-&gt;settipo($_POST['tipo']);</v>
+      </c>
+    </row>
+    <row r="8" spans="1:26" ht="72" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>120</v>
+      </c>
+      <c r="B8" t="s">
+        <v>124</v>
+      </c>
+      <c r="C8" t="str">
+        <f t="shared" si="0"/>
+        <v>$descricao,</v>
+      </c>
+      <c r="D8" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v>public function getdescricao(){
+		return $this-&gt;descricao;
+	}</v>
+      </c>
+      <c r="E8" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v>public function setdescricao($descricao){
+		$this-&gt;descricao = $descricao;
+	}</v>
+      </c>
+      <c r="F8" t="str">
+        <f t="shared" si="3"/>
+        <v>name="descricao"</v>
+      </c>
+      <c r="H8" t="str">
+        <f t="shared" si="4"/>
+        <v>$servico-&gt;setdescricao($_POST['descricao']);</v>
+      </c>
+    </row>
+    <row r="9" spans="1:26" ht="72" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>121</v>
+      </c>
+      <c r="B9" t="s">
+        <v>125</v>
+      </c>
+      <c r="C9" t="str">
+        <f t="shared" si="0"/>
+        <v>$cnpjClienteCadastro,</v>
+      </c>
+      <c r="D9" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v>public function getcnpjClienteCadastro(){
+		return $this-&gt;cnpjClienteCadastro;
+	}</v>
+      </c>
+      <c r="E9" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v>public function setcnpjClienteCadastro($cnpjClienteCadastro){
+		$this-&gt;cnpjClienteCadastro = $cnpjClienteCadastro;
+	}</v>
+      </c>
+      <c r="F9" t="str">
+        <f t="shared" si="3"/>
+        <v>name="cnpjClienteCadastro"</v>
+      </c>
+      <c r="H9" t="str">
+        <f t="shared" si="4"/>
+        <v>$servico-&gt;setcnpjClienteCadastro($_POST['cnpjClienteCadastro']);</v>
+      </c>
+    </row>
+    <row r="10" spans="1:26" ht="72" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>24</v>
+      </c>
+      <c r="B10">
+        <v>43986.545439814814</v>
+      </c>
+      <c r="C10" t="str">
+        <f t="shared" si="0"/>
+        <v>$dataCadastro,</v>
+      </c>
+      <c r="D10" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v>public function getdataCadastro(){
+		return $this-&gt;dataCadastro;
+	}</v>
+      </c>
+      <c r="E10" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v>public function setdataCadastro($dataCadastro){
+		$this-&gt;dataCadastro = $dataCadastro;
+	}</v>
+      </c>
+      <c r="F10" t="str">
+        <f t="shared" si="3"/>
+        <v>name="dataCadastro"</v>
+      </c>
+      <c r="H10" t="str">
+        <f t="shared" si="4"/>
+        <v>$servico-&gt;setdataCadastro($_POST['dataCadastro']);</v>
+      </c>
+    </row>
+    <row r="11" spans="1:26" ht="72" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>26</v>
+      </c>
+      <c r="B11">
+        <v>43986.545439814814</v>
+      </c>
+      <c r="C11" t="str">
+        <f t="shared" si="0"/>
+        <v>$dataModificacao,</v>
+      </c>
+      <c r="D11" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v>public function getdataModificacao(){
+		return $this-&gt;dataModificacao;
+	}</v>
+      </c>
+      <c r="E11" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v>public function setdataModificacao($dataModificacao){
+		$this-&gt;dataModificacao = $dataModificacao;
+	}</v>
+      </c>
+      <c r="F11" t="str">
+        <f t="shared" si="3"/>
+        <v>name="dataModificacao"</v>
+      </c>
+      <c r="H11" t="str">
+        <f t="shared" si="4"/>
+        <v>$servico-&gt;setdataModificacao($_POST['dataModificacao']);</v>
+      </c>
+    </row>
+    <row r="12" spans="1:26" ht="72" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>33</v>
+      </c>
+      <c r="B12">
+        <v>22</v>
+      </c>
+      <c r="C12" t="str">
+        <f t="shared" si="0"/>
+        <v>$idUsuario,</v>
+      </c>
+      <c r="D12" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v>public function getidUsuario(){
+		return $this-&gt;idUsuario;
+	}</v>
+      </c>
+      <c r="E12" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v>public function setidUsuario($idUsuario){
+		$this-&gt;idUsuario = $idUsuario;
+	}</v>
+      </c>
+      <c r="F12" t="str">
+        <f t="shared" si="3"/>
+        <v>name="idUsuario"</v>
+      </c>
+      <c r="H12" t="str">
+        <f t="shared" si="4"/>
+        <v>$servico-&gt;setidUsuario($_POST['idUsuario']);</v>
+      </c>
+    </row>
+    <row r="13" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="D13" s="4"/>
+      <c r="E13" s="4"/>
+    </row>
+    <row r="14" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="D14" s="4"/>
+      <c r="E14" s="4"/>
+    </row>
+    <row r="15" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="D15" s="4"/>
+      <c r="E15" s="4"/>
+    </row>
+    <row r="16" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="D16" s="4"/>
+      <c r="E16" s="4"/>
+    </row>
+    <row r="17" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="D17" s="4"/>
+      <c r="E17" s="4"/>
+    </row>
+    <row r="18" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="D18" s="4"/>
+      <c r="E18" s="4"/>
+    </row>
+    <row r="19" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="D19" s="4"/>
+      <c r="E19" s="4"/>
+    </row>
+    <row r="20" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="D20" s="4"/>
+      <c r="E20" s="4"/>
+    </row>
+    <row r="21" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="D21" s="4"/>
+      <c r="E21" s="4"/>
+    </row>
+    <row r="22" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="D22" s="4"/>
+      <c r="E22" s="4"/>
+    </row>
+    <row r="23" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="D23" s="4"/>
+      <c r="E23" s="4"/>
+    </row>
+    <row r="24" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="D24" s="4"/>
+      <c r="E24" s="4"/>
+    </row>
+    <row r="25" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="D25" s="4"/>
+      <c r="E25" s="4"/>
+    </row>
+    <row r="26" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="D26" s="4"/>
+      <c r="E26" s="4"/>
+    </row>
+    <row r="27" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="D27" s="4"/>
+      <c r="E27" s="4"/>
+    </row>
+    <row r="28" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="D28" s="4"/>
+      <c r="E28" s="4"/>
+    </row>
+    <row r="29" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="D29" s="4"/>
+      <c r="E29" s="4"/>
+    </row>
+    <row r="30" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="D30" s="4"/>
+      <c r="E30" s="4"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27F77242-1B9B-47EA-8A4A-62F783FD6B77}">
-  <dimension ref="A1:S2"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:S2"/>
+      <selection sqref="A1:H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>81</v>
+        <v>117</v>
       </c>
       <c r="B1" t="s">
-        <v>82</v>
+        <v>118</v>
       </c>
       <c r="C1" t="s">
-        <v>83</v>
+        <v>119</v>
       </c>
       <c r="D1" t="s">
-        <v>84</v>
+        <v>120</v>
       </c>
       <c r="E1" t="s">
-        <v>85</v>
+        <v>121</v>
       </c>
       <c r="F1" t="s">
-        <v>86</v>
+        <v>24</v>
       </c>
       <c r="G1" t="s">
-        <v>87</v>
+        <v>26</v>
       </c>
       <c r="H1" t="s">
-        <v>88</v>
-      </c>
-      <c r="I1" t="s">
-        <v>89</v>
-      </c>
-      <c r="J1" t="s">
-        <v>90</v>
-      </c>
-      <c r="K1" t="s">
-        <v>91</v>
-      </c>
-      <c r="L1" t="s">
-        <v>92</v>
-      </c>
-      <c r="M1" t="s">
-        <v>93</v>
-      </c>
-      <c r="N1" t="s">
-        <v>94</v>
-      </c>
-      <c r="O1" t="s">
-        <v>95</v>
-      </c>
-      <c r="P1" t="s">
-        <v>96</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>97</v>
-      </c>
-      <c r="R1" t="s">
-        <v>98</v>
-      </c>
-      <c r="S1" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>100</v>
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>18</v>
       </c>
       <c r="B2" t="s">
-        <v>101</v>
+        <v>122</v>
       </c>
       <c r="C2" t="s">
-        <v>102</v>
+        <v>123</v>
       </c>
       <c r="D2" t="s">
-        <v>103</v>
+        <v>124</v>
       </c>
       <c r="E2" t="s">
-        <v>104</v>
-      </c>
-      <c r="F2" t="s">
-        <v>105</v>
-      </c>
-      <c r="G2" t="s">
-        <v>106</v>
-      </c>
-      <c r="H2" t="s">
-        <v>107</v>
-      </c>
-      <c r="I2" t="s">
-        <v>108</v>
-      </c>
-      <c r="J2" t="s">
-        <v>109</v>
-      </c>
-      <c r="K2" t="s">
-        <v>110</v>
-      </c>
-      <c r="L2" t="s">
-        <v>111</v>
-      </c>
-      <c r="M2" t="s">
-        <v>111</v>
-      </c>
-      <c r="N2" t="s">
-        <v>112</v>
-      </c>
-      <c r="O2" t="s">
-        <v>113</v>
-      </c>
-      <c r="P2" t="s">
-        <v>114</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>114</v>
-      </c>
-      <c r="R2" t="s">
-        <v>115</v>
-      </c>
-      <c r="S2" t="s">
-        <v>116</v>
+        <v>125</v>
+      </c>
+      <c r="F2" s="2">
+        <v>43986.545439814814</v>
+      </c>
+      <c r="G2" s="2">
+        <v>43986.545439814814</v>
+      </c>
+      <c r="H2">
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
inserido o crud do cadastro de usuario
</commit_message>
<xml_diff>
--- a/documentação/Catalogo_Dados.xlsx
+++ b/documentação/Catalogo_Dados.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\projetos\contabil_novo\documentação\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD92E6D5-7CFF-462A-A683-E058B8B79343}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{373DC130-4922-4228-BCF9-8BEE12C754C8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{BBCC3619-9FAE-4B62-80B6-86EE0ECD51E8}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{BBCC3619-9FAE-4B62-80B6-86EE0ECD51E8}"/>
   </bookViews>
   <sheets>
     <sheet name="aluno" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="346" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="324" uniqueCount="127">
   <si>
     <t># id</t>
   </si>
@@ -234,54 +234,6 @@
     <t>Set Controle</t>
   </si>
   <si>
-    <t>perfil</t>
-  </si>
-  <si>
-    <t>cref</t>
-  </si>
-  <si>
-    <t>dataAdmissao</t>
-  </si>
-  <si>
-    <t>dataDemissao</t>
-  </si>
-  <si>
-    <t>login</t>
-  </si>
-  <si>
-    <t>senha</t>
-  </si>
-  <si>
-    <t>ADMINISTRADOR MORUMBI</t>
-  </si>
-  <si>
-    <t>017.570.616-65</t>
-  </si>
-  <si>
-    <t>05716-060</t>
-  </si>
-  <si>
-    <t>Rua Doutor Fonseca Brasil</t>
-  </si>
-  <si>
-    <t>Vila Andrade</t>
-  </si>
-  <si>
-    <t>(11) 3744-1221</t>
-  </si>
-  <si>
-    <t>(11) 99999-9999</t>
-  </si>
-  <si>
-    <t>teste@teste.com</t>
-  </si>
-  <si>
-    <t>usuÃ¡rio homologaÃ§Ã£o</t>
-  </si>
-  <si>
-    <t>admin</t>
-  </si>
-  <si>
     <t xml:space="preserve"> cnpj</t>
   </si>
   <si>
@@ -390,9 +342,6 @@
     <t xml:space="preserve"> razaoSocial</t>
   </si>
   <si>
-    <t># idServico</t>
-  </si>
-  <si>
     <t>servico</t>
   </si>
   <si>
@@ -415,13 +364,67 @@
   </si>
   <si>
     <t>19.313.885/0001-07</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> nome</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> sexo</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> password</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> idStatus</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> idPerfil</t>
+  </si>
+  <si>
+    <t>'1'</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'Hélio de Jesus Paiva'</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'm'</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'hjppaiva@yahoo.com.br'</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> '1'</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> '2020-07-08 12:43:29'</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ''</t>
+  </si>
+  <si>
+    <t>'2'</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'Lucia Silva'</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'f'</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'lucia.silva@gmail.com'</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> '2'</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> NULL</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -431,6 +434,14 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -464,7 +475,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -474,6 +485,7 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2260,10 +2272,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C71ECD93-53B4-4613-8409-D1464380A165}">
-  <dimension ref="A1:Z30"/>
+  <dimension ref="A1:Z14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5:E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2298,162 +2310,73 @@
   <sheetData>
     <row r="1" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>57</v>
       </c>
       <c r="B1" t="s">
-        <v>65</v>
+        <v>109</v>
       </c>
       <c r="C1" t="s">
-        <v>27</v>
+        <v>110</v>
       </c>
       <c r="D1" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="E1" t="s">
-        <v>1</v>
+        <v>111</v>
       </c>
       <c r="F1" t="s">
-        <v>2</v>
+        <v>112</v>
       </c>
       <c r="G1" t="s">
-        <v>3</v>
+        <v>113</v>
       </c>
       <c r="H1" t="s">
-        <v>4</v>
+        <v>77</v>
       </c>
       <c r="I1" t="s">
-        <v>5</v>
+        <v>78</v>
       </c>
       <c r="J1" t="s">
-        <v>6</v>
-      </c>
-      <c r="K1" t="s">
-        <v>7</v>
-      </c>
-      <c r="L1" t="s">
-        <v>8</v>
-      </c>
-      <c r="M1" t="s">
-        <v>9</v>
-      </c>
-      <c r="N1" t="s">
-        <v>10</v>
-      </c>
-      <c r="O1" t="s">
-        <v>11</v>
-      </c>
-      <c r="P1" t="s">
-        <v>12</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>13</v>
-      </c>
-      <c r="R1" t="s">
-        <v>14</v>
-      </c>
-      <c r="S1" t="s">
-        <v>67</v>
-      </c>
-      <c r="T1" t="s">
-        <v>68</v>
-      </c>
-      <c r="U1" t="s">
-        <v>22</v>
-      </c>
-      <c r="V1" t="s">
-        <v>24</v>
-      </c>
-      <c r="W1" t="s">
-        <v>25</v>
-      </c>
-      <c r="X1" t="s">
-        <v>69</v>
-      </c>
-      <c r="Y1" t="s">
-        <v>70</v>
-      </c>
-      <c r="Z1" t="s">
-        <v>26</v>
+        <v>76</v>
       </c>
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A2">
-        <v>32</v>
-      </c>
-      <c r="B2">
-        <v>1</v>
-      </c>
-      <c r="C2">
-        <v>1</v>
+      <c r="A2" t="s">
+        <v>114</v>
+      </c>
+      <c r="B2" t="s">
+        <v>115</v>
+      </c>
+      <c r="C2" t="s">
+        <v>116</v>
+      </c>
+      <c r="D2" t="s">
+        <v>117</v>
       </c>
       <c r="E2" t="s">
-        <v>71</v>
-      </c>
-      <c r="F2" s="1">
-        <v>32874</v>
-      </c>
-      <c r="G2" t="s">
-        <v>72</v>
-      </c>
-      <c r="H2">
-        <v>12345678</v>
-      </c>
-      <c r="I2">
-        <v>1</v>
+        <v>118</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="H2" t="s">
+        <v>119</v>
+      </c>
+      <c r="I2" t="s">
+        <v>119</v>
       </c>
       <c r="J2" t="s">
-        <v>73</v>
-      </c>
-      <c r="K2" t="s">
-        <v>74</v>
-      </c>
-      <c r="L2" t="s">
-        <v>75</v>
-      </c>
-      <c r="M2" t="s">
-        <v>41</v>
-      </c>
-      <c r="N2" t="s">
-        <v>42</v>
-      </c>
-      <c r="O2">
-        <v>253</v>
-      </c>
-      <c r="P2" t="s">
-        <v>76</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>77</v>
-      </c>
-      <c r="R2" t="s">
-        <v>78</v>
-      </c>
-      <c r="S2" s="1">
-        <v>36526</v>
-      </c>
-      <c r="T2" t="s">
-        <v>54</v>
-      </c>
-      <c r="U2" t="s">
-        <v>79</v>
-      </c>
-      <c r="V2" s="2">
-        <v>42857.439814814818</v>
-      </c>
-      <c r="W2" t="s">
-        <v>52</v>
-      </c>
-      <c r="X2" t="s">
-        <v>80</v>
-      </c>
-      <c r="Y2">
-        <v>452458</v>
-      </c>
-      <c r="Z2" s="2">
-        <v>42857.439814814818</v>
-      </c>
+        <v>120</v>
+      </c>
+      <c r="S2" s="1"/>
+      <c r="V2" s="2"/>
+      <c r="Z2" s="2"/>
     </row>
     <row r="3" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A3" s="7"/>
       <c r="F3" s="1"/>
       <c r="S3" s="1"/>
       <c r="V3" s="2"/>
@@ -2485,15 +2408,15 @@
         <v>64</v>
       </c>
     </row>
-    <row r="5" spans="1:26" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:26" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>57</v>
       </c>
-      <c r="B5">
-        <v>32</v>
+      <c r="B5" t="s">
+        <v>114</v>
       </c>
       <c r="C5" t="str">
-        <f t="shared" ref="C5:C30" si="0">"$"&amp;A5&amp;","</f>
+        <f>"$"&amp;TRIM(A5)&amp;","</f>
         <v>$id,</v>
       </c>
       <c r="D5" s="4" t="str">
@@ -2523,803 +2446,294 @@
     </row>
     <row r="6" spans="1:26" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>65</v>
-      </c>
-      <c r="B6">
-        <v>1</v>
+        <v>109</v>
+      </c>
+      <c r="B6" t="s">
+        <v>115</v>
       </c>
       <c r="C6" t="str">
-        <f t="shared" si="0"/>
-        <v>$perfil,</v>
+        <f t="shared" ref="C6:C14" si="0">"$"&amp;TRIM(A6)&amp;","</f>
+        <v>$nome,</v>
       </c>
       <c r="D6" s="4" t="str">
-        <f t="shared" ref="D6:D30" si="1">"public function get"&amp;$A6&amp;"(){
+        <f t="shared" ref="D6:D14" si="1">"public function get"&amp;$A6&amp;"(){
 		return $this-&gt;"&amp;$A6&amp;";
 	}"</f>
-        <v>public function getperfil(){
-		return $this-&gt;perfil;
+        <v>public function get nome(){
+		return $this-&gt; nome;
 	}</v>
       </c>
       <c r="E6" s="4" t="str">
-        <f t="shared" ref="E6:E30" si="2">"public function set"&amp;$A6&amp;"($"&amp;A6&amp;"){
+        <f t="shared" ref="E6:E14" si="2">"public function set"&amp;$A6&amp;"($"&amp;A6&amp;"){
 		$this-&gt;"&amp;$A6&amp;" = $"&amp;A6&amp;";
 	}"</f>
-        <v>public function setperfil($perfil){
-		$this-&gt;perfil = $perfil;
+        <v>public function set nome($ nome){
+		$this-&gt; nome = $ nome;
 	}</v>
       </c>
       <c r="F6" t="str">
-        <f t="shared" ref="F6:F30" si="3">"name="""&amp;A6&amp;""""</f>
-        <v>name="perfil"</v>
+        <f t="shared" ref="F6:F14" si="3">"name="""&amp;A6&amp;""""</f>
+        <v>name=" nome"</v>
       </c>
       <c r="H6" t="str">
-        <f t="shared" ref="H6:H30" si="4">"$usuario-&gt;set"&amp;$A6&amp;"($_POST['"&amp;$A6&amp;"']);"</f>
-        <v>$usuario-&gt;setperfil($_POST['perfil']);</v>
+        <f t="shared" ref="H6:H14" si="4">"$usuario-&gt;set"&amp;$A6&amp;"($_POST['"&amp;$A6&amp;"']);"</f>
+        <v>$usuario-&gt;set nome($_POST[' nome']);</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>27</v>
-      </c>
-      <c r="B7">
-        <v>1</v>
+        <v>110</v>
+      </c>
+      <c r="B7" t="s">
+        <v>116</v>
       </c>
       <c r="C7" t="str">
         <f t="shared" si="0"/>
-        <v>$idUnidade,</v>
+        <v>$sexo,</v>
       </c>
       <c r="D7" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>public function getidUnidade(){
-		return $this-&gt;idUnidade;
+        <v>public function get sexo(){
+		return $this-&gt; sexo;
 	}</v>
       </c>
       <c r="E7" s="4" t="str">
         <f t="shared" si="2"/>
-        <v>public function setidUnidade($idUnidade){
-		$this-&gt;idUnidade = $idUnidade;
+        <v>public function set sexo($ sexo){
+		$this-&gt; sexo = $ sexo;
 	}</v>
       </c>
       <c r="F7" t="str">
         <f t="shared" si="3"/>
-        <v>name="idUnidade"</v>
+        <v>name=" sexo"</v>
       </c>
       <c r="H7" t="str">
         <f t="shared" si="4"/>
-        <v>$usuario-&gt;setidUnidade($_POST['idUnidade']);</v>
+        <v>$usuario-&gt;set sexo($_POST[' sexo']);</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>66</v>
+        <v>72</v>
+      </c>
+      <c r="B8" t="s">
+        <v>117</v>
       </c>
       <c r="C8" t="str">
         <f t="shared" si="0"/>
-        <v>$cref,</v>
+        <v>$email,</v>
       </c>
       <c r="D8" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>public function getcref(){
-		return $this-&gt;cref;
+        <v>public function get email(){
+		return $this-&gt; email;
 	}</v>
       </c>
       <c r="E8" s="4" t="str">
         <f t="shared" si="2"/>
-        <v>public function setcref($cref){
-		$this-&gt;cref = $cref;
+        <v>public function set email($ email){
+		$this-&gt; email = $ email;
 	}</v>
       </c>
       <c r="F8" t="str">
         <f t="shared" si="3"/>
-        <v>name="cref"</v>
+        <v>name=" email"</v>
       </c>
       <c r="H8" t="str">
         <f t="shared" si="4"/>
-        <v>$usuario-&gt;setcref($_POST['cref']);</v>
+        <v>$usuario-&gt;set email($_POST[' email']);</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>1</v>
+        <v>111</v>
       </c>
       <c r="B9" t="s">
-        <v>71</v>
+        <v>118</v>
       </c>
       <c r="C9" t="str">
         <f t="shared" si="0"/>
-        <v>$nome,</v>
+        <v>$password,</v>
       </c>
       <c r="D9" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>public function getnome(){
-		return $this-&gt;nome;
+        <v>public function get password(){
+		return $this-&gt; password;
 	}</v>
       </c>
       <c r="E9" s="4" t="str">
         <f t="shared" si="2"/>
-        <v>public function setnome($nome){
-		$this-&gt;nome = $nome;
+        <v>public function set password($ password){
+		$this-&gt; password = $ password;
 	}</v>
       </c>
       <c r="F9" t="str">
         <f t="shared" si="3"/>
-        <v>name="nome"</v>
+        <v>name=" password"</v>
       </c>
       <c r="H9" t="str">
         <f t="shared" si="4"/>
-        <v>$usuario-&gt;setnome($_POST['nome']);</v>
+        <v>$usuario-&gt;set password($_POST[' password']);</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>2</v>
-      </c>
-      <c r="B10">
-        <v>32874</v>
+        <v>112</v>
+      </c>
+      <c r="B10" t="s">
+        <v>118</v>
       </c>
       <c r="C10" t="str">
         <f t="shared" si="0"/>
-        <v>$dataNascimento,</v>
+        <v>$idStatus,</v>
       </c>
       <c r="D10" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>public function getdataNascimento(){
-		return $this-&gt;dataNascimento;
+        <v>public function get idStatus(){
+		return $this-&gt; idStatus;
 	}</v>
       </c>
       <c r="E10" s="4" t="str">
         <f t="shared" si="2"/>
-        <v>public function setdataNascimento($dataNascimento){
-		$this-&gt;dataNascimento = $dataNascimento;
+        <v>public function set idStatus($ idStatus){
+		$this-&gt; idStatus = $ idStatus;
 	}</v>
       </c>
       <c r="F10" t="str">
         <f t="shared" si="3"/>
-        <v>name="dataNascimento"</v>
+        <v>name=" idStatus"</v>
       </c>
       <c r="H10" t="str">
         <f t="shared" si="4"/>
-        <v>$usuario-&gt;setdataNascimento($_POST['dataNascimento']);</v>
+        <v>$usuario-&gt;set idStatus($_POST[' idStatus']);</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>3</v>
+        <v>113</v>
       </c>
       <c r="B11" t="s">
-        <v>72</v>
+        <v>118</v>
       </c>
       <c r="C11" t="str">
         <f t="shared" si="0"/>
-        <v>$cpf,</v>
+        <v>$idPerfil,</v>
       </c>
       <c r="D11" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>public function getcpf(){
-		return $this-&gt;cpf;
+        <v>public function get idPerfil(){
+		return $this-&gt; idPerfil;
 	}</v>
       </c>
       <c r="E11" s="4" t="str">
         <f t="shared" si="2"/>
-        <v>public function setcpf($cpf){
-		$this-&gt;cpf = $cpf;
+        <v>public function set idPerfil($ idPerfil){
+		$this-&gt; idPerfil = $ idPerfil;
 	}</v>
       </c>
       <c r="F11" t="str">
         <f t="shared" si="3"/>
-        <v>name="cpf"</v>
+        <v>name=" idPerfil"</v>
       </c>
       <c r="H11" t="str">
         <f t="shared" si="4"/>
-        <v>$usuario-&gt;setcpf($_POST['cpf']);</v>
+        <v>$usuario-&gt;set idPerfil($_POST[' idPerfil']);</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>4</v>
-      </c>
-      <c r="B12">
-        <v>12345678</v>
+        <v>77</v>
+      </c>
+      <c r="B12" t="s">
+        <v>119</v>
       </c>
       <c r="C12" t="str">
         <f t="shared" si="0"/>
-        <v>$rg,</v>
+        <v>$dataCadastro,</v>
       </c>
       <c r="D12" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>public function getrg(){
-		return $this-&gt;rg;
+        <v>public function get dataCadastro(){
+		return $this-&gt; dataCadastro;
 	}</v>
       </c>
       <c r="E12" s="4" t="str">
         <f t="shared" si="2"/>
-        <v>public function setrg($rg){
-		$this-&gt;rg = $rg;
+        <v>public function set dataCadastro($ dataCadastro){
+		$this-&gt; dataCadastro = $ dataCadastro;
 	}</v>
       </c>
       <c r="F12" t="str">
         <f t="shared" si="3"/>
-        <v>name="rg"</v>
+        <v>name=" dataCadastro"</v>
       </c>
       <c r="H12" t="str">
         <f t="shared" si="4"/>
-        <v>$usuario-&gt;setrg($_POST['rg']);</v>
+        <v>$usuario-&gt;set dataCadastro($_POST[' dataCadastro']);</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>5</v>
-      </c>
-      <c r="B13">
-        <v>1</v>
+        <v>78</v>
+      </c>
+      <c r="B13" t="s">
+        <v>119</v>
       </c>
       <c r="C13" t="str">
         <f t="shared" si="0"/>
-        <v>$sexo,</v>
+        <v>$dataModificacao,</v>
       </c>
       <c r="D13" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>public function getsexo(){
-		return $this-&gt;sexo;
+        <v>public function get dataModificacao(){
+		return $this-&gt; dataModificacao;
 	}</v>
       </c>
       <c r="E13" s="4" t="str">
         <f t="shared" si="2"/>
-        <v>public function setsexo($sexo){
-		$this-&gt;sexo = $sexo;
+        <v>public function set dataModificacao($ dataModificacao){
+		$this-&gt; dataModificacao = $ dataModificacao;
 	}</v>
       </c>
       <c r="F13" t="str">
         <f t="shared" si="3"/>
-        <v>name="sexo"</v>
+        <v>name=" dataModificacao"</v>
       </c>
       <c r="H13" t="str">
         <f t="shared" si="4"/>
-        <v>$usuario-&gt;setsexo($_POST['sexo']);</v>
-      </c>
-    </row>
-    <row r="14" spans="1:26" ht="57.6" x14ac:dyDescent="0.3">
+        <v>$usuario-&gt;set dataModificacao($_POST[' dataModificacao']);</v>
+      </c>
+    </row>
+    <row r="14" spans="1:26" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>6</v>
+        <v>76</v>
       </c>
       <c r="B14" t="s">
-        <v>73</v>
+        <v>120</v>
       </c>
       <c r="C14" t="str">
         <f t="shared" si="0"/>
-        <v>$cep,</v>
+        <v>$obs,</v>
       </c>
       <c r="D14" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>public function getcep(){
-		return $this-&gt;cep;
+        <v>public function get obs(){
+		return $this-&gt; obs;
 	}</v>
       </c>
       <c r="E14" s="4" t="str">
         <f t="shared" si="2"/>
-        <v>public function setcep($cep){
-		$this-&gt;cep = $cep;
+        <v>public function set obs($ obs){
+		$this-&gt; obs = $ obs;
 	}</v>
       </c>
       <c r="F14" t="str">
         <f t="shared" si="3"/>
-        <v>name="cep"</v>
+        <v>name=" obs"</v>
       </c>
       <c r="H14" t="str">
         <f t="shared" si="4"/>
-        <v>$usuario-&gt;setcep($_POST['cep']);</v>
-      </c>
-    </row>
-    <row r="15" spans="1:26" ht="72" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
-        <v>7</v>
-      </c>
-      <c r="B15" t="s">
-        <v>74</v>
-      </c>
-      <c r="C15" t="str">
-        <f t="shared" si="0"/>
-        <v>$endereco,</v>
-      </c>
-      <c r="D15" s="4" t="str">
-        <f t="shared" si="1"/>
-        <v>public function getendereco(){
-		return $this-&gt;endereco;
-	}</v>
-      </c>
-      <c r="E15" s="4" t="str">
-        <f t="shared" si="2"/>
-        <v>public function setendereco($endereco){
-		$this-&gt;endereco = $endereco;
-	}</v>
-      </c>
-      <c r="F15" t="str">
-        <f t="shared" si="3"/>
-        <v>name="endereco"</v>
-      </c>
-      <c r="H15" t="str">
-        <f t="shared" si="4"/>
-        <v>$usuario-&gt;setendereco($_POST['endereco']);</v>
-      </c>
-    </row>
-    <row r="16" spans="1:26" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
-        <v>8</v>
-      </c>
-      <c r="B16" t="s">
-        <v>75</v>
-      </c>
-      <c r="C16" t="str">
-        <f t="shared" si="0"/>
-        <v>$bairro,</v>
-      </c>
-      <c r="D16" s="4" t="str">
-        <f t="shared" si="1"/>
-        <v>public function getbairro(){
-		return $this-&gt;bairro;
-	}</v>
-      </c>
-      <c r="E16" s="4" t="str">
-        <f t="shared" si="2"/>
-        <v>public function setbairro($bairro){
-		$this-&gt;bairro = $bairro;
-	}</v>
-      </c>
-      <c r="F16" t="str">
-        <f t="shared" si="3"/>
-        <v>name="bairro"</v>
-      </c>
-      <c r="H16" t="str">
-        <f t="shared" si="4"/>
-        <v>$usuario-&gt;setbairro($_POST['bairro']);</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" ht="72" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
-        <v>9</v>
-      </c>
-      <c r="B17" t="s">
-        <v>41</v>
-      </c>
-      <c r="C17" t="str">
-        <f t="shared" si="0"/>
-        <v>$cidade,</v>
-      </c>
-      <c r="D17" s="4" t="str">
-        <f t="shared" si="1"/>
-        <v>public function getcidade(){
-		return $this-&gt;cidade;
-	}</v>
-      </c>
-      <c r="E17" s="4" t="str">
-        <f t="shared" si="2"/>
-        <v>public function setcidade($cidade){
-		$this-&gt;cidade = $cidade;
-	}</v>
-      </c>
-      <c r="F17" t="str">
-        <f t="shared" si="3"/>
-        <v>name="cidade"</v>
-      </c>
-      <c r="H17" t="str">
-        <f t="shared" si="4"/>
-        <v>$usuario-&gt;setcidade($_POST['cidade']);</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
-        <v>10</v>
-      </c>
-      <c r="B18" t="s">
-        <v>42</v>
-      </c>
-      <c r="C18" t="str">
-        <f t="shared" si="0"/>
-        <v>$uf,</v>
-      </c>
-      <c r="D18" s="4" t="str">
-        <f t="shared" si="1"/>
-        <v>public function getuf(){
-		return $this-&gt;uf;
-	}</v>
-      </c>
-      <c r="E18" s="4" t="str">
-        <f t="shared" si="2"/>
-        <v>public function setuf($uf){
-		$this-&gt;uf = $uf;
-	}</v>
-      </c>
-      <c r="F18" t="str">
-        <f t="shared" si="3"/>
-        <v>name="uf"</v>
-      </c>
-      <c r="H18" t="str">
-        <f t="shared" si="4"/>
-        <v>$usuario-&gt;setuf($_POST['uf']);</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" ht="72" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
-        <v>11</v>
-      </c>
-      <c r="B19">
-        <v>253</v>
-      </c>
-      <c r="C19" t="str">
-        <f t="shared" si="0"/>
-        <v>$numero,</v>
-      </c>
-      <c r="D19" s="4" t="str">
-        <f t="shared" si="1"/>
-        <v>public function getnumero(){
-		return $this-&gt;numero;
-	}</v>
-      </c>
-      <c r="E19" s="4" t="str">
-        <f t="shared" si="2"/>
-        <v>public function setnumero($numero){
-		$this-&gt;numero = $numero;
-	}</v>
-      </c>
-      <c r="F19" t="str">
-        <f t="shared" si="3"/>
-        <v>name="numero"</v>
-      </c>
-      <c r="H19" t="str">
-        <f t="shared" si="4"/>
-        <v>$usuario-&gt;setnumero($_POST['numero']);</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" ht="72" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
-        <v>12</v>
-      </c>
-      <c r="B20" t="s">
-        <v>76</v>
-      </c>
-      <c r="C20" t="str">
-        <f t="shared" si="0"/>
-        <v>$telefone,</v>
-      </c>
-      <c r="D20" s="4" t="str">
-        <f t="shared" si="1"/>
-        <v>public function gettelefone(){
-		return $this-&gt;telefone;
-	}</v>
-      </c>
-      <c r="E20" s="4" t="str">
-        <f t="shared" si="2"/>
-        <v>public function settelefone($telefone){
-		$this-&gt;telefone = $telefone;
-	}</v>
-      </c>
-      <c r="F20" t="str">
-        <f t="shared" si="3"/>
-        <v>name="telefone"</v>
-      </c>
-      <c r="H20" t="str">
-        <f t="shared" si="4"/>
-        <v>$usuario-&gt;settelefone($_POST['telefone']);</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" ht="72" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
-        <v>13</v>
-      </c>
-      <c r="B21" t="s">
-        <v>77</v>
-      </c>
-      <c r="C21" t="str">
-        <f t="shared" si="0"/>
-        <v>$celular,</v>
-      </c>
-      <c r="D21" s="4" t="str">
-        <f t="shared" si="1"/>
-        <v>public function getcelular(){
-		return $this-&gt;celular;
-	}</v>
-      </c>
-      <c r="E21" s="4" t="str">
-        <f t="shared" si="2"/>
-        <v>public function setcelular($celular){
-		$this-&gt;celular = $celular;
-	}</v>
-      </c>
-      <c r="F21" t="str">
-        <f t="shared" si="3"/>
-        <v>name="celular"</v>
-      </c>
-      <c r="H21" t="str">
-        <f t="shared" si="4"/>
-        <v>$usuario-&gt;setcelular($_POST['celular']);</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
-        <v>14</v>
-      </c>
-      <c r="B22" t="s">
-        <v>78</v>
-      </c>
-      <c r="C22" t="str">
-        <f t="shared" si="0"/>
-        <v>$email,</v>
-      </c>
-      <c r="D22" s="4" t="str">
-        <f t="shared" si="1"/>
-        <v>public function getemail(){
-		return $this-&gt;email;
-	}</v>
-      </c>
-      <c r="E22" s="4" t="str">
-        <f t="shared" si="2"/>
-        <v>public function setemail($email){
-		$this-&gt;email = $email;
-	}</v>
-      </c>
-      <c r="F22" t="str">
-        <f t="shared" si="3"/>
-        <v>name="email"</v>
-      </c>
-      <c r="H22" t="str">
-        <f t="shared" si="4"/>
-        <v>$usuario-&gt;setemail($_POST['email']);</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A23" t="s">
-        <v>67</v>
-      </c>
-      <c r="B23">
-        <v>36526</v>
-      </c>
-      <c r="C23" t="str">
-        <f t="shared" si="0"/>
-        <v>$dataAdmissao,</v>
-      </c>
-      <c r="D23" s="4" t="str">
-        <f t="shared" si="1"/>
-        <v>public function getdataAdmissao(){
-		return $this-&gt;dataAdmissao;
-	}</v>
-      </c>
-      <c r="E23" s="4" t="str">
-        <f t="shared" si="2"/>
-        <v>public function setdataAdmissao($dataAdmissao){
-		$this-&gt;dataAdmissao = $dataAdmissao;
-	}</v>
-      </c>
-      <c r="F23" t="str">
-        <f t="shared" si="3"/>
-        <v>name="dataAdmissao"</v>
-      </c>
-      <c r="H23" t="str">
-        <f t="shared" si="4"/>
-        <v>$usuario-&gt;setdataAdmissao($_POST['dataAdmissao']);</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A24" t="s">
-        <v>68</v>
-      </c>
-      <c r="B24" t="s">
-        <v>54</v>
-      </c>
-      <c r="C24" t="str">
-        <f t="shared" si="0"/>
-        <v>$dataDemissao,</v>
-      </c>
-      <c r="D24" s="4" t="str">
-        <f t="shared" si="1"/>
-        <v>public function getdataDemissao(){
-		return $this-&gt;dataDemissao;
-	}</v>
-      </c>
-      <c r="E24" s="4" t="str">
-        <f t="shared" si="2"/>
-        <v>public function setdataDemissao($dataDemissao){
-		$this-&gt;dataDemissao = $dataDemissao;
-	}</v>
-      </c>
-      <c r="F24" t="str">
-        <f t="shared" si="3"/>
-        <v>name="dataDemissao"</v>
-      </c>
-      <c r="H24" t="str">
-        <f t="shared" si="4"/>
-        <v>$usuario-&gt;setdataDemissao($_POST['dataDemissao']);</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A25" t="s">
-        <v>22</v>
-      </c>
-      <c r="B25" t="s">
-        <v>79</v>
-      </c>
-      <c r="C25" t="str">
-        <f t="shared" si="0"/>
-        <v>$observacao,</v>
-      </c>
-      <c r="D25" s="4" t="str">
-        <f t="shared" si="1"/>
-        <v>public function getobservacao(){
-		return $this-&gt;observacao;
-	}</v>
-      </c>
-      <c r="E25" s="4" t="str">
-        <f t="shared" si="2"/>
-        <v>public function setobservacao($observacao){
-		$this-&gt;observacao = $observacao;
-	}</v>
-      </c>
-      <c r="F25" t="str">
-        <f t="shared" si="3"/>
-        <v>name="observacao"</v>
-      </c>
-      <c r="H25" t="str">
-        <f t="shared" si="4"/>
-        <v>$usuario-&gt;setobservacao($_POST['observacao']);</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A26" t="s">
-        <v>24</v>
-      </c>
-      <c r="B26">
-        <v>42857.439814814818</v>
-      </c>
-      <c r="C26" t="str">
-        <f t="shared" si="0"/>
-        <v>$dataCadastro,</v>
-      </c>
-      <c r="D26" s="4" t="str">
-        <f t="shared" si="1"/>
-        <v>public function getdataCadastro(){
-		return $this-&gt;dataCadastro;
-	}</v>
-      </c>
-      <c r="E26" s="4" t="str">
-        <f t="shared" si="2"/>
-        <v>public function setdataCadastro($dataCadastro){
-		$this-&gt;dataCadastro = $dataCadastro;
-	}</v>
-      </c>
-      <c r="F26" t="str">
-        <f t="shared" si="3"/>
-        <v>name="dataCadastro"</v>
-      </c>
-      <c r="H26" t="str">
-        <f t="shared" si="4"/>
-        <v>$usuario-&gt;setdataCadastro($_POST['dataCadastro']);</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A27" t="s">
-        <v>25</v>
-      </c>
-      <c r="B27" t="s">
-        <v>52</v>
-      </c>
-      <c r="C27" t="str">
-        <f t="shared" si="0"/>
-        <v>$status,</v>
-      </c>
-      <c r="D27" s="4" t="str">
-        <f t="shared" si="1"/>
-        <v>public function getstatus(){
-		return $this-&gt;status;
-	}</v>
-      </c>
-      <c r="E27" s="4" t="str">
-        <f t="shared" si="2"/>
-        <v>public function setstatus($status){
-		$this-&gt;status = $status;
-	}</v>
-      </c>
-      <c r="F27" t="str">
-        <f t="shared" si="3"/>
-        <v>name="status"</v>
-      </c>
-      <c r="H27" t="str">
-        <f t="shared" si="4"/>
-        <v>$usuario-&gt;setstatus($_POST['status']);</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A28" t="s">
-        <v>69</v>
-      </c>
-      <c r="B28" t="s">
-        <v>80</v>
-      </c>
-      <c r="C28" t="str">
-        <f t="shared" si="0"/>
-        <v>$login,</v>
-      </c>
-      <c r="D28" s="4" t="str">
-        <f t="shared" si="1"/>
-        <v>public function getlogin(){
-		return $this-&gt;login;
-	}</v>
-      </c>
-      <c r="E28" s="4" t="str">
-        <f t="shared" si="2"/>
-        <v>public function setlogin($login){
-		$this-&gt;login = $login;
-	}</v>
-      </c>
-      <c r="F28" t="str">
-        <f t="shared" si="3"/>
-        <v>name="login"</v>
-      </c>
-      <c r="H28" t="str">
-        <f t="shared" si="4"/>
-        <v>$usuario-&gt;setlogin($_POST['login']);</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A29" t="s">
-        <v>70</v>
-      </c>
-      <c r="B29">
-        <v>452458</v>
-      </c>
-      <c r="C29" t="str">
-        <f t="shared" si="0"/>
-        <v>$senha,</v>
-      </c>
-      <c r="D29" s="4" t="str">
-        <f t="shared" si="1"/>
-        <v>public function getsenha(){
-		return $this-&gt;senha;
-	}</v>
-      </c>
-      <c r="E29" s="4" t="str">
-        <f t="shared" si="2"/>
-        <v>public function setsenha($senha){
-		$this-&gt;senha = $senha;
-	}</v>
-      </c>
-      <c r="F29" t="str">
-        <f t="shared" si="3"/>
-        <v>name="senha"</v>
-      </c>
-      <c r="H29" t="str">
-        <f t="shared" si="4"/>
-        <v>$usuario-&gt;setsenha($_POST['senha']);</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A30" t="s">
-        <v>26</v>
-      </c>
-      <c r="B30">
-        <v>42857.439814814818</v>
-      </c>
-      <c r="C30" t="str">
-        <f t="shared" si="0"/>
-        <v>$dataModificacao,</v>
-      </c>
-      <c r="D30" s="4" t="str">
-        <f t="shared" si="1"/>
-        <v>public function getdataModificacao(){
-		return $this-&gt;dataModificacao;
-	}</v>
-      </c>
-      <c r="E30" s="4" t="str">
-        <f t="shared" si="2"/>
-        <v>public function setdataModificacao($dataModificacao){
-		$this-&gt;dataModificacao = $dataModificacao;
-	}</v>
-      </c>
-      <c r="F30" t="str">
-        <f t="shared" si="3"/>
-        <v>name="dataModificacao"</v>
-      </c>
-      <c r="H30" t="str">
-        <f t="shared" si="4"/>
-        <v>$usuario-&gt;setdataModificacao($_POST['dataModificacao']);</v>
+        <v>$usuario-&gt;set obs($_POST[' obs']);</v>
       </c>
     </row>
   </sheetData>
@@ -3367,120 +2781,120 @@
   <sheetData>
     <row r="1" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>114</v>
+        <v>98</v>
       </c>
       <c r="B1" t="s">
-        <v>81</v>
+        <v>65</v>
       </c>
       <c r="C1" t="s">
-        <v>115</v>
+        <v>99</v>
       </c>
       <c r="D1" t="s">
-        <v>116</v>
+        <v>100</v>
       </c>
       <c r="E1" t="s">
-        <v>82</v>
+        <v>66</v>
       </c>
       <c r="F1" t="s">
-        <v>83</v>
+        <v>67</v>
       </c>
       <c r="G1" t="s">
-        <v>84</v>
+        <v>68</v>
       </c>
       <c r="H1" t="s">
-        <v>85</v>
+        <v>69</v>
       </c>
       <c r="I1" t="s">
-        <v>86</v>
+        <v>70</v>
       </c>
       <c r="J1" t="s">
-        <v>87</v>
+        <v>71</v>
       </c>
       <c r="K1" t="s">
-        <v>88</v>
+        <v>72</v>
       </c>
       <c r="L1" t="s">
-        <v>89</v>
+        <v>73</v>
       </c>
       <c r="M1" t="s">
-        <v>90</v>
+        <v>74</v>
       </c>
       <c r="N1" t="s">
-        <v>91</v>
+        <v>75</v>
       </c>
       <c r="O1" t="s">
-        <v>92</v>
+        <v>76</v>
       </c>
       <c r="P1" t="s">
-        <v>93</v>
+        <v>77</v>
       </c>
       <c r="Q1" t="s">
-        <v>94</v>
+        <v>78</v>
       </c>
       <c r="R1" t="s">
-        <v>95</v>
+        <v>79</v>
       </c>
       <c r="S1" t="s">
-        <v>96</v>
+        <v>80</v>
       </c>
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>81</v>
+      </c>
+      <c r="B2" t="s">
+        <v>82</v>
+      </c>
+      <c r="C2" t="s">
+        <v>83</v>
+      </c>
+      <c r="D2" t="s">
+        <v>84</v>
+      </c>
+      <c r="E2" t="s">
+        <v>85</v>
+      </c>
+      <c r="F2" t="s">
+        <v>86</v>
+      </c>
+      <c r="G2" t="s">
+        <v>87</v>
+      </c>
+      <c r="H2" t="s">
+        <v>88</v>
+      </c>
+      <c r="I2" t="s">
+        <v>89</v>
+      </c>
+      <c r="J2" t="s">
+        <v>90</v>
+      </c>
+      <c r="K2" t="s">
+        <v>91</v>
+      </c>
+      <c r="L2" t="s">
+        <v>92</v>
+      </c>
+      <c r="M2" t="s">
+        <v>92</v>
+      </c>
+      <c r="N2" t="s">
+        <v>93</v>
+      </c>
+      <c r="O2" t="s">
+        <v>94</v>
+      </c>
+      <c r="P2" t="s">
+        <v>95</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>95</v>
+      </c>
+      <c r="R2" t="s">
+        <v>96</v>
+      </c>
+      <c r="S2" t="s">
         <v>97</v>
-      </c>
-      <c r="B2" t="s">
-        <v>98</v>
-      </c>
-      <c r="C2" t="s">
-        <v>99</v>
-      </c>
-      <c r="D2" t="s">
-        <v>100</v>
-      </c>
-      <c r="E2" t="s">
-        <v>101</v>
-      </c>
-      <c r="F2" t="s">
-        <v>102</v>
-      </c>
-      <c r="G2" t="s">
-        <v>103</v>
-      </c>
-      <c r="H2" t="s">
-        <v>104</v>
-      </c>
-      <c r="I2" t="s">
-        <v>105</v>
-      </c>
-      <c r="J2" t="s">
-        <v>106</v>
-      </c>
-      <c r="K2" t="s">
-        <v>107</v>
-      </c>
-      <c r="L2" t="s">
-        <v>108</v>
-      </c>
-      <c r="M2" t="s">
-        <v>108</v>
-      </c>
-      <c r="N2" t="s">
-        <v>109</v>
-      </c>
-      <c r="O2" t="s">
-        <v>110</v>
-      </c>
-      <c r="P2" t="s">
-        <v>111</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>111</v>
-      </c>
-      <c r="R2" t="s">
-        <v>112</v>
-      </c>
-      <c r="S2" t="s">
-        <v>113</v>
       </c>
       <c r="V2" s="2"/>
       <c r="Z2" s="2"/>
@@ -3519,10 +2933,10 @@
     </row>
     <row r="5" spans="1:26" ht="72" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>114</v>
+        <v>98</v>
       </c>
       <c r="B5" t="s">
-        <v>97</v>
+        <v>81</v>
       </c>
       <c r="C5" t="str">
         <f>"$"&amp;TRIM(A5)&amp;","</f>
@@ -3555,10 +2969,10 @@
     </row>
     <row r="6" spans="1:26" ht="72" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>81</v>
+        <v>65</v>
       </c>
       <c r="B6" t="s">
-        <v>98</v>
+        <v>82</v>
       </c>
       <c r="C6" t="str">
         <f t="shared" ref="C6:C23" si="0">"$"&amp;TRIM(A6)&amp;","</f>
@@ -3591,10 +3005,10 @@
     </row>
     <row r="7" spans="1:26" ht="72" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>115</v>
+        <v>99</v>
       </c>
       <c r="B7" t="s">
-        <v>99</v>
+        <v>83</v>
       </c>
       <c r="C7" t="str">
         <f t="shared" si="0"/>
@@ -3623,10 +3037,10 @@
     </row>
     <row r="8" spans="1:26" ht="72" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>116</v>
+        <v>100</v>
       </c>
       <c r="B8" t="s">
-        <v>100</v>
+        <v>84</v>
       </c>
       <c r="C8" t="str">
         <f t="shared" si="0"/>
@@ -3655,10 +3069,10 @@
     </row>
     <row r="9" spans="1:26" ht="72" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>82</v>
+        <v>66</v>
       </c>
       <c r="B9" t="s">
-        <v>101</v>
+        <v>85</v>
       </c>
       <c r="C9" t="str">
         <f t="shared" si="0"/>
@@ -3687,10 +3101,10 @@
     </row>
     <row r="10" spans="1:26" ht="72" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>83</v>
+        <v>67</v>
       </c>
       <c r="B10" t="s">
-        <v>102</v>
+        <v>86</v>
       </c>
       <c r="C10" t="str">
         <f t="shared" si="0"/>
@@ -3719,10 +3133,10 @@
     </row>
     <row r="11" spans="1:26" ht="72" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>84</v>
+        <v>68</v>
       </c>
       <c r="B11" t="s">
-        <v>103</v>
+        <v>87</v>
       </c>
       <c r="C11" t="str">
         <f t="shared" si="0"/>
@@ -3751,10 +3165,10 @@
     </row>
     <row r="12" spans="1:26" ht="72" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>85</v>
+        <v>69</v>
       </c>
       <c r="B12" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
       <c r="C12" t="str">
         <f t="shared" si="0"/>
@@ -3783,10 +3197,10 @@
     </row>
     <row r="13" spans="1:26" ht="72" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>86</v>
+        <v>70</v>
       </c>
       <c r="B13" t="s">
-        <v>105</v>
+        <v>89</v>
       </c>
       <c r="C13" t="str">
         <f t="shared" si="0"/>
@@ -3815,10 +3229,10 @@
     </row>
     <row r="14" spans="1:26" ht="72" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>87</v>
+        <v>71</v>
       </c>
       <c r="B14" t="s">
-        <v>106</v>
+        <v>90</v>
       </c>
       <c r="C14" t="str">
         <f t="shared" si="0"/>
@@ -3847,10 +3261,10 @@
     </row>
     <row r="15" spans="1:26" ht="72" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>88</v>
+        <v>72</v>
       </c>
       <c r="B15" t="s">
-        <v>107</v>
+        <v>91</v>
       </c>
       <c r="C15" t="str">
         <f t="shared" si="0"/>
@@ -3879,10 +3293,10 @@
     </row>
     <row r="16" spans="1:26" ht="72" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>89</v>
+        <v>73</v>
       </c>
       <c r="B16" t="s">
-        <v>108</v>
+        <v>92</v>
       </c>
       <c r="C16" t="str">
         <f t="shared" si="0"/>
@@ -3911,10 +3325,10 @@
     </row>
     <row r="17" spans="1:8" ht="72" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>90</v>
+        <v>74</v>
       </c>
       <c r="B17" t="s">
-        <v>108</v>
+        <v>92</v>
       </c>
       <c r="C17" t="str">
         <f t="shared" si="0"/>
@@ -3943,10 +3357,10 @@
     </row>
     <row r="18" spans="1:8" ht="72" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>91</v>
+        <v>75</v>
       </c>
       <c r="B18" t="s">
-        <v>109</v>
+        <v>93</v>
       </c>
       <c r="C18" t="str">
         <f t="shared" si="0"/>
@@ -3975,10 +3389,10 @@
     </row>
     <row r="19" spans="1:8" ht="72" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>92</v>
+        <v>76</v>
       </c>
       <c r="B19" t="s">
-        <v>110</v>
+        <v>94</v>
       </c>
       <c r="C19" t="str">
         <f t="shared" si="0"/>
@@ -4007,10 +3421,10 @@
     </row>
     <row r="20" spans="1:8" ht="72" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>93</v>
+        <v>77</v>
       </c>
       <c r="B20" t="s">
-        <v>111</v>
+        <v>95</v>
       </c>
       <c r="C20" t="str">
         <f t="shared" si="0"/>
@@ -4039,10 +3453,10 @@
     </row>
     <row r="21" spans="1:8" ht="72" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>94</v>
+        <v>78</v>
       </c>
       <c r="B21" t="s">
-        <v>111</v>
+        <v>95</v>
       </c>
       <c r="C21" t="str">
         <f t="shared" si="0"/>
@@ -4071,10 +3485,10 @@
     </row>
     <row r="22" spans="1:8" ht="72" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>95</v>
+        <v>79</v>
       </c>
       <c r="B22" t="s">
-        <v>112</v>
+        <v>96</v>
       </c>
       <c r="C22" t="str">
         <f t="shared" si="0"/>
@@ -4103,10 +3517,10 @@
     </row>
     <row r="23" spans="1:8" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>96</v>
+        <v>80</v>
       </c>
       <c r="B23" t="s">
-        <v>113</v>
+        <v>97</v>
       </c>
       <c r="C23" t="str">
         <f t="shared" si="0"/>
@@ -4170,7 +3584,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68FFEDBE-4954-4567-A0F1-2F9B239AEB62}">
   <dimension ref="A1:Z30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+    <sheetView topLeftCell="C1" workbookViewId="0">
       <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
@@ -4209,16 +3623,16 @@
         <v>57</v>
       </c>
       <c r="B1" t="s">
-        <v>118</v>
+        <v>101</v>
       </c>
       <c r="C1" t="s">
-        <v>119</v>
+        <v>102</v>
       </c>
       <c r="D1" t="s">
-        <v>120</v>
+        <v>103</v>
       </c>
       <c r="E1" t="s">
-        <v>121</v>
+        <v>104</v>
       </c>
       <c r="F1" t="s">
         <v>24</v>
@@ -4235,16 +3649,16 @@
         <v>18</v>
       </c>
       <c r="B2" t="s">
-        <v>122</v>
+        <v>105</v>
       </c>
       <c r="C2" t="s">
-        <v>123</v>
+        <v>106</v>
       </c>
       <c r="D2" t="s">
-        <v>124</v>
+        <v>107</v>
       </c>
       <c r="E2" t="s">
-        <v>125</v>
+        <v>108</v>
       </c>
       <c r="F2" s="2">
         <v>43986.545439814814</v>
@@ -4328,17 +3742,17 @@
     </row>
     <row r="6" spans="1:26" ht="72" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>118</v>
+        <v>101</v>
       </c>
       <c r="B6" t="s">
-        <v>122</v>
+        <v>105</v>
       </c>
       <c r="C6" t="str">
-        <f t="shared" ref="C6:C23" si="0">"$"&amp;TRIM(A6)&amp;","</f>
+        <f t="shared" ref="C6:C12" si="0">"$"&amp;TRIM(A6)&amp;","</f>
         <v>$servico,</v>
       </c>
       <c r="D6" s="4" t="str">
-        <f t="shared" ref="D6:D23" si="1">"public function get"&amp;TRIM($A6)&amp;"(){
+        <f t="shared" ref="D6:D12" si="1">"public function get"&amp;TRIM($A6)&amp;"(){
 		return $this-&gt;"&amp;TRIM($A6)&amp;";
 	}"</f>
         <v>public function getservico(){
@@ -4346,7 +3760,7 @@
 	}</v>
       </c>
       <c r="E6" s="4" t="str">
-        <f t="shared" ref="E6:E23" si="2">"public function set"&amp;TRIM($A6)&amp;"($"&amp;TRIM(A6)&amp;"){
+        <f t="shared" ref="E6:E12" si="2">"public function set"&amp;TRIM($A6)&amp;"($"&amp;TRIM(A6)&amp;"){
 		$this-&gt;"&amp;TRIM($A6)&amp;" = $"&amp;TRIM(A6)&amp;";
 	}"</f>
         <v>public function setservico($servico){
@@ -4354,7 +3768,7 @@
 	}</v>
       </c>
       <c r="F6" t="str">
-        <f t="shared" ref="F6:F23" si="3">"name="""&amp;A6&amp;""""</f>
+        <f t="shared" ref="F6:F12" si="3">"name="""&amp;A6&amp;""""</f>
         <v>name="servico"</v>
       </c>
       <c r="H6" t="str">
@@ -4364,10 +3778,10 @@
     </row>
     <row r="7" spans="1:26" ht="72" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>119</v>
+        <v>102</v>
       </c>
       <c r="B7" t="s">
-        <v>123</v>
+        <v>106</v>
       </c>
       <c r="C7" t="str">
         <f t="shared" si="0"/>
@@ -4396,10 +3810,10 @@
     </row>
     <row r="8" spans="1:26" ht="72" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>120</v>
+        <v>103</v>
       </c>
       <c r="B8" t="s">
-        <v>124</v>
+        <v>107</v>
       </c>
       <c r="C8" t="str">
         <f t="shared" si="0"/>
@@ -4428,10 +3842,10 @@
     </row>
     <row r="9" spans="1:26" ht="72" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>121</v>
+        <v>104</v>
       </c>
       <c r="B9" t="s">
-        <v>125</v>
+        <v>108</v>
       </c>
       <c r="C9" t="str">
         <f t="shared" si="0"/>
@@ -4458,7 +3872,7 @@
         <v>$servico-&gt;setcnpjClienteCadastro($_POST['cnpjClienteCadastro']);</v>
       </c>
     </row>
-    <row r="10" spans="1:26" ht="72" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:26" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>24</v>
       </c>
@@ -4490,7 +3904,7 @@
         <v>$servico-&gt;setdataCadastro($_POST['dataCadastro']);</v>
       </c>
     </row>
-    <row r="11" spans="1:26" ht="72" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:26" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>26</v>
       </c>
@@ -4633,64 +4047,119 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27F77242-1B9B-47EA-8A4A-62F783FD6B77}">
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:J3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:H2"/>
+      <selection sqref="A1:J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="3.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.21875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.21875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.88671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="19.44140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="5.88671875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B1" t="s">
+        <v>109</v>
+      </c>
+      <c r="C1" t="s">
+        <v>110</v>
+      </c>
+      <c r="D1" t="s">
+        <v>72</v>
+      </c>
+      <c r="E1" t="s">
+        <v>111</v>
+      </c>
+      <c r="F1" t="s">
+        <v>112</v>
+      </c>
+      <c r="G1" t="s">
+        <v>113</v>
+      </c>
+      <c r="H1" t="s">
+        <v>77</v>
+      </c>
+      <c r="I1" t="s">
+        <v>78</v>
+      </c>
+      <c r="J1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>114</v>
+      </c>
+      <c r="B2" t="s">
+        <v>115</v>
+      </c>
+      <c r="C2" t="s">
+        <v>116</v>
+      </c>
+      <c r="D2" t="s">
         <v>117</v>
       </c>
-      <c r="B1" t="s">
+      <c r="E2" t="s">
         <v>118</v>
       </c>
-      <c r="C1" t="s">
+      <c r="F2" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="H2" t="s">
         <v>119</v>
       </c>
-      <c r="D1" t="s">
+      <c r="I2" t="s">
+        <v>119</v>
+      </c>
+      <c r="J2" t="s">
         <v>120</v>
       </c>
-      <c r="E1" t="s">
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
         <v>121</v>
       </c>
-      <c r="F1" t="s">
-        <v>24</v>
-      </c>
-      <c r="G1" t="s">
-        <v>26</v>
-      </c>
-      <c r="H1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A2">
-        <v>18</v>
-      </c>
-      <c r="B2" t="s">
+      <c r="B3" t="s">
         <v>122</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C3" t="s">
         <v>123</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D3" t="s">
         <v>124</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E3" t="s">
+        <v>118</v>
+      </c>
+      <c r="F3" t="s">
+        <v>118</v>
+      </c>
+      <c r="G3" t="s">
         <v>125</v>
       </c>
-      <c r="F2" s="2">
-        <v>43986.545439814814</v>
-      </c>
-      <c r="G2" s="2">
-        <v>43986.545439814814</v>
-      </c>
-      <c r="H2">
-        <v>22</v>
+      <c r="H3" t="s">
+        <v>119</v>
+      </c>
+      <c r="I3" t="s">
+        <v>119</v>
+      </c>
+      <c r="J3" t="s">
+        <v>126</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
inserido o crud do cadastro de lancamento
</commit_message>
<xml_diff>
--- a/documentação/Catalogo_Dados.xlsx
+++ b/documentação/Catalogo_Dados.xlsx
@@ -8,16 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\projetos\contabil_novo\documentação\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{373DC130-4922-4228-BCF9-8BEE12C754C8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81EBA5E4-39E0-49E3-8FE3-09750D6620E1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{BBCC3619-9FAE-4B62-80B6-86EE0ECD51E8}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="4" xr2:uid="{BBCC3619-9FAE-4B62-80B6-86EE0ECD51E8}"/>
   </bookViews>
   <sheets>
     <sheet name="aluno" sheetId="1" r:id="rId1"/>
     <sheet name="usuario" sheetId="2" r:id="rId2"/>
     <sheet name="cliente" sheetId="3" r:id="rId3"/>
     <sheet name="servico" sheetId="5" r:id="rId4"/>
-    <sheet name="Planilha2" sheetId="4" r:id="rId5"/>
+    <sheet name="lancamento" sheetId="6" r:id="rId5"/>
+    <sheet name="Planilha2" sheetId="4" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="324" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="354" uniqueCount="132">
   <si>
     <t># id</t>
   </si>
@@ -418,6 +419,21 @@
   </si>
   <si>
     <t xml:space="preserve"> NULL</t>
+  </si>
+  <si>
+    <t>valor</t>
+  </si>
+  <si>
+    <t>dataVencimento</t>
+  </si>
+  <si>
+    <t>pago</t>
+  </si>
+  <si>
+    <t>Entrada</t>
+  </si>
+  <si>
+    <t>150.98</t>
   </si>
 </sst>
 </file>
@@ -2274,7 +2290,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C71ECD93-53B4-4613-8409-D1464380A165}">
   <dimension ref="A1:Z14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+    <sheetView topLeftCell="A9" workbookViewId="0">
       <selection activeCell="E5" sqref="E5:E14"/>
     </sheetView>
   </sheetViews>
@@ -2444,7 +2460,7 @@
         <v>$usuario-&gt;setid($_POST['id']);</v>
       </c>
     </row>
-    <row r="6" spans="1:26" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:26" ht="72" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>109</v>
       </c>
@@ -3584,8 +3600,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68FFEDBE-4954-4567-A0F1-2F9B239AEB62}">
   <dimension ref="A1:Z30"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4046,6 +4062,373 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AAEA5B6A-037B-497B-8C39-BCE2D0A2890B}">
+  <dimension ref="A1:H12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="15" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.77734375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="50.88671875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B1" t="s">
+        <v>103</v>
+      </c>
+      <c r="C1" t="s">
+        <v>102</v>
+      </c>
+      <c r="D1" t="s">
+        <v>127</v>
+      </c>
+      <c r="E1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G1" t="s">
+        <v>128</v>
+      </c>
+      <c r="H1" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>105</v>
+      </c>
+      <c r="C2" t="s">
+        <v>130</v>
+      </c>
+      <c r="D2" t="s">
+        <v>131</v>
+      </c>
+      <c r="E2" s="2">
+        <v>43986.545439814814</v>
+      </c>
+      <c r="F2" s="2">
+        <v>43986.545439814814</v>
+      </c>
+      <c r="G2" s="2">
+        <v>43986.545439814814</v>
+      </c>
+      <c r="H2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A4" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>57</v>
+      </c>
+      <c r="B5">
+        <v>2</v>
+      </c>
+      <c r="C5" t="str">
+        <f>"$"&amp;TRIM(A5)&amp;","</f>
+        <v>$id,</v>
+      </c>
+      <c r="D5" s="4" t="str">
+        <f>"public function get"&amp;TRIM($A5)&amp;"(){
+		return $this-&gt;"&amp;TRIM($A5)&amp;";
+	}"</f>
+        <v>public function getid(){
+		return $this-&gt;id;
+	}</v>
+      </c>
+      <c r="E5" s="4" t="str">
+        <f>"public function set"&amp;TRIM($A5)&amp;"($"&amp;TRIM(A5)&amp;"){
+		$this-&gt;"&amp;TRIM($A5)&amp;" = $"&amp;TRIM(A5)&amp;";
+	}"</f>
+        <v>public function setid($id){
+		$this-&gt;id = $id;
+	}</v>
+      </c>
+      <c r="F5" t="str">
+        <f>"name="""&amp;A5&amp;""""</f>
+        <v>name="id"</v>
+      </c>
+      <c r="H5" t="str">
+        <f>"$lancamento-&gt;set"&amp;$A5&amp;"($_POST['"&amp;$A5&amp;"']);"</f>
+        <v>$lancamento-&gt;setid($_POST['id']);</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>103</v>
+      </c>
+      <c r="B6" t="s">
+        <v>105</v>
+      </c>
+      <c r="C6" t="str">
+        <f t="shared" ref="C6:C12" si="0">"$"&amp;TRIM(A6)&amp;","</f>
+        <v>$descricao,</v>
+      </c>
+      <c r="D6" s="4" t="str">
+        <f t="shared" ref="D6:D12" si="1">"public function get"&amp;TRIM($A6)&amp;"(){
+		return $this-&gt;"&amp;TRIM($A6)&amp;";
+	}"</f>
+        <v>public function getdescricao(){
+		return $this-&gt;descricao;
+	}</v>
+      </c>
+      <c r="E6" s="4" t="str">
+        <f t="shared" ref="E6:E12" si="2">"public function set"&amp;TRIM($A6)&amp;"($"&amp;TRIM(A6)&amp;"){
+		$this-&gt;"&amp;TRIM($A6)&amp;" = $"&amp;TRIM(A6)&amp;";
+	}"</f>
+        <v>public function setdescricao($descricao){
+		$this-&gt;descricao = $descricao;
+	}</v>
+      </c>
+      <c r="F6" t="str">
+        <f t="shared" ref="F6:F12" si="3">"name="""&amp;A6&amp;""""</f>
+        <v>name="descricao"</v>
+      </c>
+      <c r="H6" t="str">
+        <f t="shared" ref="H6:H12" si="4">"$lancamento-&gt;set"&amp;$A6&amp;"($_POST['"&amp;$A6&amp;"']);"</f>
+        <v>$lancamento-&gt;setdescricao($_POST['descricao']);</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>102</v>
+      </c>
+      <c r="B7" t="s">
+        <v>130</v>
+      </c>
+      <c r="C7" t="str">
+        <f t="shared" si="0"/>
+        <v>$tipo,</v>
+      </c>
+      <c r="D7" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v>public function gettipo(){
+		return $this-&gt;tipo;
+	}</v>
+      </c>
+      <c r="E7" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v>public function settipo($tipo){
+		$this-&gt;tipo = $tipo;
+	}</v>
+      </c>
+      <c r="F7" t="str">
+        <f t="shared" si="3"/>
+        <v>name="tipo"</v>
+      </c>
+      <c r="H7" t="str">
+        <f t="shared" si="4"/>
+        <v>$lancamento-&gt;settipo($_POST['tipo']);</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>127</v>
+      </c>
+      <c r="B8" t="s">
+        <v>131</v>
+      </c>
+      <c r="C8" t="str">
+        <f t="shared" si="0"/>
+        <v>$valor,</v>
+      </c>
+      <c r="D8" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v>public function getvalor(){
+		return $this-&gt;valor;
+	}</v>
+      </c>
+      <c r="E8" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v>public function setvalor($valor){
+		$this-&gt;valor = $valor;
+	}</v>
+      </c>
+      <c r="F8" t="str">
+        <f t="shared" si="3"/>
+        <v>name="valor"</v>
+      </c>
+      <c r="H8" t="str">
+        <f t="shared" si="4"/>
+        <v>$lancamento-&gt;setvalor($_POST['valor']);</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="144" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>24</v>
+      </c>
+      <c r="B9">
+        <v>43986.545439814814</v>
+      </c>
+      <c r="C9" t="str">
+        <f t="shared" si="0"/>
+        <v>$dataCadastro,</v>
+      </c>
+      <c r="D9" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v>public function getdataCadastro(){
+		return $this-&gt;dataCadastro;
+	}</v>
+      </c>
+      <c r="E9" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v>public function setdataCadastro($dataCadastro){
+		$this-&gt;dataCadastro = $dataCadastro;
+	}</v>
+      </c>
+      <c r="F9" t="str">
+        <f t="shared" si="3"/>
+        <v>name="dataCadastro"</v>
+      </c>
+      <c r="H9" t="str">
+        <f t="shared" si="4"/>
+        <v>$lancamento-&gt;setdataCadastro($_POST['dataCadastro']);</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>26</v>
+      </c>
+      <c r="B10">
+        <v>43986.545439814814</v>
+      </c>
+      <c r="C10" t="str">
+        <f t="shared" si="0"/>
+        <v>$dataModificacao,</v>
+      </c>
+      <c r="D10" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v>public function getdataModificacao(){
+		return $this-&gt;dataModificacao;
+	}</v>
+      </c>
+      <c r="E10" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v>public function setdataModificacao($dataModificacao){
+		$this-&gt;dataModificacao = $dataModificacao;
+	}</v>
+      </c>
+      <c r="F10" t="str">
+        <f t="shared" si="3"/>
+        <v>name="dataModificacao"</v>
+      </c>
+      <c r="H10" t="str">
+        <f t="shared" si="4"/>
+        <v>$lancamento-&gt;setdataModificacao($_POST['dataModificacao']);</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>128</v>
+      </c>
+      <c r="B11">
+        <v>43986.545439814814</v>
+      </c>
+      <c r="C11" t="str">
+        <f t="shared" si="0"/>
+        <v>$dataVencimento,</v>
+      </c>
+      <c r="D11" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v>public function getdataVencimento(){
+		return $this-&gt;dataVencimento;
+	}</v>
+      </c>
+      <c r="E11" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v>public function setdataVencimento($dataVencimento){
+		$this-&gt;dataVencimento = $dataVencimento;
+	}</v>
+      </c>
+      <c r="F11" t="str">
+        <f t="shared" si="3"/>
+        <v>name="dataVencimento"</v>
+      </c>
+      <c r="H11" t="str">
+        <f t="shared" si="4"/>
+        <v>$lancamento-&gt;setdataVencimento($_POST['dataVencimento']);</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>129</v>
+      </c>
+      <c r="B12">
+        <v>1</v>
+      </c>
+      <c r="C12" t="str">
+        <f t="shared" si="0"/>
+        <v>$pago,</v>
+      </c>
+      <c r="D12" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v>public function getpago(){
+		return $this-&gt;pago;
+	}</v>
+      </c>
+      <c r="E12" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v>public function setpago($pago){
+		$this-&gt;pago = $pago;
+	}</v>
+      </c>
+      <c r="F12" t="str">
+        <f t="shared" si="3"/>
+        <v>name="pago"</v>
+      </c>
+      <c r="H12" t="str">
+        <f t="shared" si="4"/>
+        <v>$lancamento-&gt;setpago($_POST['pago']);</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27F77242-1B9B-47EA-8A4A-62F783FD6B77}">
   <dimension ref="A1:J3"/>
   <sheetViews>

</xml_diff>